<commit_message>
Add led array holder BOM tab.
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,17 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{061EDFE6-5D40-6E45-BAA7-E763A1C111C8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A8226B-066C-E048-B34F-EE5078BB5DC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33840" windowHeight="21580" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33840" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept Estimate" sheetId="1" r:id="rId1"/>
     <sheet name="Core Board V0.3" sheetId="2" r:id="rId2"/>
     <sheet name="Logic Board V0.3" sheetId="3" r:id="rId3"/>
+    <sheet name="Middle Layers" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Core Board V0.3'!$A$6:$M$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Middle Layers'!$A$6:$M$31</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="450">
   <si>
     <t>Digi-Key Part Number</t>
   </si>
@@ -1361,6 +1363,36 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Stylus</t>
+  </si>
+  <si>
+    <t>Stylus magnet sphere</t>
+  </si>
+  <si>
+    <t>Stylus plug</t>
+  </si>
+  <si>
+    <t>3D printed LED Array holder</t>
+  </si>
+  <si>
+    <t>LED Array</t>
+  </si>
+  <si>
+    <t>stylus rention magnet</t>
+  </si>
+  <si>
+    <t>stylus friction o-ring</t>
+  </si>
+  <si>
+    <t>Diffuser layer</t>
+  </si>
+  <si>
+    <t>Screen protector layer</t>
+  </si>
+  <si>
+    <t>Pimoroni Unicorn Hat</t>
   </si>
 </sst>
 </file>
@@ -1372,10 +1404,17 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1499,36 +1538,36 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="3" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1538,53 +1577,65 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4341,7 +4392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5DBFB5-E21A-7B4B-815F-748A526FD280}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="125" workbookViewId="0">
       <selection activeCell="P8" sqref="P8:P12"/>
     </sheetView>
   </sheetViews>
@@ -4383,45 +4434,45 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="30" t="s">
+      <c r="O3" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="30"/>
-      <c r="Q3" s="30"/>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
       <c r="B4" s="27"/>
-      <c r="J4" s="31" t="s">
+      <c r="J4" s="30" t="s">
         <v>175</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="30" t="s">
         <v>176</v>
       </c>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
     </row>
     <row r="5" spans="1:17" ht="34" x14ac:dyDescent="0.15">
-      <c r="B5" s="31" t="s">
+      <c r="B5" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="30" t="s">
         <v>179</v>
       </c>
       <c r="I5" s="28" t="s">
         <v>180</v>
       </c>
-      <c r="J5" s="42" t="s">
+      <c r="J5" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="41" t="s">
         <v>182</v>
       </c>
       <c r="L5" s="28" t="s">
@@ -4468,10 +4519,10 @@
       <c r="I6" s="28" t="s">
         <v>194</v>
       </c>
-      <c r="J6" s="42" t="s">
+      <c r="J6" s="41" t="s">
         <v>195</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="K6" s="41" t="s">
         <v>196</v>
       </c>
       <c r="L6" s="28" t="s">
@@ -4518,7 +4569,7 @@
       <c r="I7" s="28">
         <v>2</v>
       </c>
-      <c r="J7" s="31">
+      <c r="J7" s="30">
         <f>IF(I7&gt;D7,0,D7-I7)</f>
         <v>6</v>
       </c>
@@ -4534,7 +4585,7 @@
         <f t="shared" ref="M7:M24" si="1">(4*D7)-L7</f>
         <v>32</v>
       </c>
-      <c r="Q7" s="33" t="e">
+      <c r="Q7" s="32" t="e">
         <f t="shared" ref="Q7:Q9" si="2">P7/O7</f>
         <v>#DIV/0!</v>
       </c>
@@ -4567,7 +4618,7 @@
       <c r="I8" s="28">
         <v>1</v>
       </c>
-      <c r="J8" s="31">
+      <c r="J8" s="30">
         <v>10</v>
       </c>
       <c r="K8" s="28">
@@ -4582,7 +4633,7 @@
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="Q8" s="33" t="e">
+      <c r="Q8" s="32" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -4591,13 +4642,13 @@
       <c r="A9" s="28">
         <v>103</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>210</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="31">
+      <c r="D9" s="30">
         <v>70</v>
       </c>
       <c r="E9" s="28" t="s">
@@ -4632,7 +4683,7 @@
         <f t="shared" si="1"/>
         <v>-580</v>
       </c>
-      <c r="Q9" s="33" t="e">
+      <c r="Q9" s="32" t="e">
         <f t="shared" si="2"/>
         <v>#DIV/0!</v>
       </c>
@@ -4641,13 +4692,13 @@
       <c r="A10" s="28">
         <v>102</v>
       </c>
-      <c r="B10" s="31" t="s">
+      <c r="B10" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="C10" s="31" t="s">
+      <c r="C10" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="D10" s="31">
+      <c r="D10" s="30">
         <v>0.8</v>
       </c>
       <c r="E10" s="28" t="s">
@@ -4685,7 +4736,7 @@
       <c r="O10" s="28">
         <v>430</v>
       </c>
-      <c r="Q10" s="33">
+      <c r="Q10" s="32">
         <f>P10/O10</f>
         <v>0</v>
       </c>
@@ -4694,13 +4745,13 @@
       <c r="A11" s="28">
         <v>103</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>214</v>
       </c>
-      <c r="D11" s="31">
+      <c r="D11" s="30">
         <v>0.8</v>
       </c>
       <c r="E11" s="28" t="s">
@@ -4715,10 +4766,10 @@
       <c r="H11" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="I11" s="34">
-        <v>0</v>
-      </c>
-      <c r="J11" s="35">
+      <c r="I11" s="33">
+        <v>0</v>
+      </c>
+      <c r="J11" s="34">
         <v>100</v>
       </c>
       <c r="K11" s="28">
@@ -4736,10 +4787,10 @@
       <c r="O11" s="28">
         <v>100</v>
       </c>
-      <c r="P11" s="36">
+      <c r="P11" s="35">
         <v>6.49</v>
       </c>
-      <c r="Q11" s="33">
+      <c r="Q11" s="32">
         <f>P11/O11</f>
         <v>6.4899999999999999E-2</v>
       </c>
@@ -4748,13 +4799,13 @@
       <c r="A12" s="28">
         <v>103</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="30" t="s">
         <v>213</v>
       </c>
-      <c r="C12" s="31" t="s">
+      <c r="C12" s="30" t="s">
         <v>220</v>
       </c>
-      <c r="D12" s="31">
+      <c r="D12" s="30">
         <v>0.75</v>
       </c>
       <c r="E12" s="28" t="s">
@@ -4769,10 +4820,10 @@
       <c r="H12" s="28" t="s">
         <v>206</v>
       </c>
-      <c r="I12" s="34">
-        <v>0</v>
-      </c>
-      <c r="J12" s="35">
+      <c r="I12" s="33">
+        <v>0</v>
+      </c>
+      <c r="J12" s="34">
         <f>2450/3.281</f>
         <v>746.72355989027733</v>
       </c>
@@ -4791,11 +4842,11 @@
       <c r="O12" s="28">
         <v>747</v>
       </c>
-      <c r="P12" s="36">
+      <c r="P12" s="35">
         <f>12.65+3.95+1.18</f>
         <v>17.78</v>
       </c>
-      <c r="Q12" s="33">
+      <c r="Q12" s="32">
         <f>P12/O12</f>
         <v>2.3801874163319948E-2</v>
       </c>
@@ -4810,7 +4861,7 @@
       <c r="C13" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="D13" s="31">
+      <c r="D13" s="30">
         <v>2</v>
       </c>
       <c r="E13" s="28" t="s">
@@ -4825,7 +4876,7 @@
       <c r="I13" s="28">
         <v>0</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="30">
         <f t="shared" ref="J13:J24" si="4">IF(I13&gt;D13,0,D13-I13)</f>
         <v>2</v>
       </c>
@@ -4841,7 +4892,7 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="Q13" s="33" t="e">
+      <c r="Q13" s="32" t="e">
         <f t="shared" ref="Q13:Q24" si="5">P13/O13</f>
         <v>#DIV/0!</v>
       </c>
@@ -4887,7 +4938,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q14" s="33" t="e">
+      <c r="Q14" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -4902,7 +4953,7 @@
       <c r="C15" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="D15" s="31">
+      <c r="D15" s="30">
         <v>1</v>
       </c>
       <c r="E15" s="28" t="s">
@@ -4936,7 +4987,7 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q15" s="33" t="e">
+      <c r="Q15" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -4982,7 +5033,7 @@
         <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="Q16" s="33" t="e">
+      <c r="Q16" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -4997,7 +5048,7 @@
       <c r="C17" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="D17" s="31">
+      <c r="D17" s="30">
         <v>1</v>
       </c>
       <c r="E17" s="28" t="s">
@@ -5028,7 +5079,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q17" s="33" t="e">
+      <c r="Q17" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -5043,7 +5094,7 @@
       <c r="C18" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="D18" s="31">
+      <c r="D18" s="30">
         <v>2</v>
       </c>
       <c r="E18" s="28" t="s">
@@ -5074,7 +5125,7 @@
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="Q18" s="33" t="e">
+      <c r="Q18" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -5089,7 +5140,7 @@
       <c r="C19" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="D19" s="31">
+      <c r="D19" s="30">
         <v>1</v>
       </c>
       <c r="E19" s="28" t="s">
@@ -5120,7 +5171,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q19" s="33" t="e">
+      <c r="Q19" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -5135,7 +5186,7 @@
       <c r="C20" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="D20" s="31">
+      <c r="D20" s="30">
         <v>1</v>
       </c>
       <c r="E20" s="28" t="s">
@@ -5166,7 +5217,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q20" s="33" t="e">
+      <c r="Q20" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -5181,7 +5232,7 @@
       <c r="C21" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="D21" s="31">
+      <c r="D21" s="30">
         <v>1</v>
       </c>
       <c r="E21" s="28" t="s">
@@ -5212,7 +5263,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q21" s="33" t="e">
+      <c r="Q21" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -5227,7 +5278,7 @@
       <c r="C22" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="D22" s="31">
+      <c r="D22" s="30">
         <v>1</v>
       </c>
       <c r="E22" s="28" t="s">
@@ -5258,7 +5309,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q22" s="33" t="e">
+      <c r="Q22" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -5273,7 +5324,7 @@
       <c r="C23" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="D23" s="31">
+      <c r="D23" s="30">
         <v>1</v>
       </c>
       <c r="E23" s="28" t="s">
@@ -5304,7 +5355,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q23" s="33" t="e">
+      <c r="Q23" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -5319,7 +5370,7 @@
       <c r="C24" s="28" t="s">
         <v>252</v>
       </c>
-      <c r="D24" s="31">
+      <c r="D24" s="30">
         <v>1</v>
       </c>
       <c r="E24" s="28" t="s">
@@ -5350,7 +5401,7 @@
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="Q24" s="33" t="e">
+      <c r="Q24" s="32" t="e">
         <f t="shared" si="5"/>
         <v>#DIV/0!</v>
       </c>
@@ -5407,110 +5458,110 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="R7" sqref="R7"/>
+    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59:XFD59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="37"/>
-    <col min="2" max="2" width="40.6640625" style="37" customWidth="1"/>
-    <col min="3" max="3" width="27" style="38" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="37"/>
+    <col min="1" max="1" width="10.83203125" style="36"/>
+    <col min="2" max="2" width="40.6640625" style="36" customWidth="1"/>
+    <col min="3" max="3" width="27" style="37" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="36"/>
     <col min="5" max="5" width="5.83203125" style="28" customWidth="1"/>
-    <col min="6" max="7" width="27" style="38" customWidth="1"/>
-    <col min="8" max="8" width="11" style="37" customWidth="1"/>
-    <col min="9" max="9" width="25" style="37" customWidth="1"/>
-    <col min="10" max="13" width="11.6640625" style="37" customWidth="1"/>
-    <col min="14" max="14" width="5.1640625" style="37" customWidth="1"/>
+    <col min="6" max="7" width="27" style="37" customWidth="1"/>
+    <col min="8" max="8" width="11" style="36" customWidth="1"/>
+    <col min="9" max="9" width="25" style="36" customWidth="1"/>
+    <col min="10" max="13" width="11.6640625" style="36" customWidth="1"/>
+    <col min="14" max="14" width="5.1640625" style="36" customWidth="1"/>
     <col min="15" max="15" width="16.33203125" style="28" customWidth="1"/>
     <col min="16" max="16" width="10.83203125" style="28"/>
     <col min="17" max="17" width="9.1640625" style="28" customWidth="1"/>
-    <col min="18" max="18" width="57" style="37" customWidth="1"/>
-    <col min="19" max="16384" width="10.83203125" style="37"/>
+    <col min="18" max="18" width="57" style="36" customWidth="1"/>
+    <col min="19" max="16384" width="10.83203125" style="36"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="36" t="s">
         <v>254</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="36" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="36" t="s">
         <v>256</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="36" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="36" t="s">
         <v>258</v>
       </c>
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="36" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" s="37" t="s">
+      <c r="A4" s="36" t="s">
         <v>260</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="36" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" s="37" t="s">
+      <c r="A5" s="36" t="s">
         <v>262</v>
       </c>
-      <c r="B5" s="37">
+      <c r="B5" s="36">
         <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" s="37" t="s">
+      <c r="A6" s="36" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="O7" s="30" t="s">
+      <c r="O7" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="42"/>
     </row>
     <row r="8" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="37" t="s">
+      <c r="A8" s="36" t="s">
         <v>264</v>
       </c>
       <c r="I8" s="28"/>
-      <c r="J8" s="31" t="s">
+      <c r="J8" s="30" t="s">
         <v>265</v>
       </c>
-      <c r="K8" s="31" t="s">
+      <c r="K8" s="30" t="s">
         <v>176</v>
       </c>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
       <c r="N8" s="28"/>
-      <c r="O8" s="32"/>
-      <c r="P8" s="32"/>
-      <c r="Q8" s="32"/>
+      <c r="O8" s="31"/>
+      <c r="P8" s="31"/>
+      <c r="Q8" s="31"/>
     </row>
     <row r="9" spans="1:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="30" t="s">
         <v>177</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="30" t="s">
         <v>178</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="30" t="s">
         <v>179</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="30" t="s">
         <v>179</v>
       </c>
       <c r="G9" s="28"/>
@@ -5541,28 +5592,28 @@
       </c>
     </row>
     <row r="10" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="37" t="s">
+      <c r="A10" s="36" t="s">
         <v>439</v>
       </c>
-      <c r="B10" s="38" t="s">
+      <c r="B10" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="C10" s="37" t="s">
+      <c r="C10" s="36" t="s">
         <v>266</v>
       </c>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="38" t="s">
         <v>267</v>
       </c>
       <c r="E10" s="28" t="s">
         <v>191</v>
       </c>
-      <c r="F10" s="37" t="s">
+      <c r="F10" s="36" t="s">
         <v>268</v>
       </c>
       <c r="G10" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="H10" s="37" t="s">
+      <c r="H10" s="36" t="s">
         <v>269</v>
       </c>
       <c r="I10" s="28" t="s">
@@ -5590,76 +5641,76 @@
       <c r="Q10" s="28" t="s">
         <v>200</v>
       </c>
-      <c r="R10" s="37" t="s">
+      <c r="R10" s="36" t="s">
         <v>270</v>
       </c>
-      <c r="S10" s="37" t="s">
+      <c r="S10" s="36" t="s">
         <v>271</v>
       </c>
-      <c r="T10" s="37" t="s">
+      <c r="T10" s="36" t="s">
         <v>272</v>
       </c>
-      <c r="U10" s="37" t="s">
+      <c r="U10" s="36" t="s">
         <v>273</v>
       </c>
-      <c r="V10" s="37" t="s">
+      <c r="V10" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="W10" s="37" t="s">
+      <c r="W10" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="X10" s="37" t="s">
+      <c r="X10" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="Y10" s="37" t="s">
+      <c r="Y10" s="36" t="s">
         <v>276</v>
       </c>
-      <c r="Z10" s="37" t="s">
+      <c r="Z10" s="36" t="s">
         <v>277</v>
       </c>
-      <c r="AA10" s="37" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB10" s="37" t="s">
+      <c r="AA10" s="36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="36" t="s">
         <v>278</v>
       </c>
-      <c r="AC10" s="37" t="s">
+      <c r="AC10" s="36" t="s">
         <v>279</v>
       </c>
-      <c r="AD10" s="37" t="s">
+      <c r="AD10" s="36" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A11" s="37">
-        <v>1</v>
-      </c>
-      <c r="B11" s="38" t="s">
+      <c r="A11" s="36">
+        <v>1</v>
+      </c>
+      <c r="B11" s="37" t="s">
         <v>281</v>
       </c>
-      <c r="C11" s="37" t="s">
+      <c r="C11" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="D11" s="39">
+      <c r="D11" s="38">
         <v>2</v>
       </c>
       <c r="E11" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F11" s="37" t="s">
+      <c r="F11" s="36" t="s">
         <v>283</v>
       </c>
-      <c r="G11" s="37" t="s">
+      <c r="G11" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="H11" s="37" t="s">
+      <c r="H11" s="36" t="s">
         <v>206</v>
       </c>
       <c r="I11" s="28">
         <v>0</v>
       </c>
-      <c r="J11" s="31">
-        <f t="shared" ref="J11:J57" si="0">IF(I11&gt;D11,0,D11-I11)</f>
+      <c r="J11" s="30">
+        <f>IF(I11&gt;D11,0,D11-I11)</f>
         <v>2</v>
       </c>
       <c r="K11" s="28">
@@ -5671,788 +5722,788 @@
         <v>0</v>
       </c>
       <c r="M11" s="28">
-        <f t="shared" ref="M11:M62" si="1">(4*D11)-L11</f>
+        <f>(4*D11)-L11</f>
         <v>8</v>
       </c>
       <c r="N11" s="28"/>
-      <c r="Q11" s="33" t="e">
-        <f t="shared" ref="Q11:Q13" si="2">P11/O11</f>
+      <c r="Q11" s="32" t="e">
+        <f>P11/O11</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R11" s="37" t="s">
+      <c r="R11" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="S11" s="37" t="s">
+      <c r="S11" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="12" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="37">
+      <c r="A12" s="36">
         <v>2</v>
       </c>
-      <c r="B12" s="38" t="s">
+      <c r="B12" s="37" t="s">
         <v>287</v>
       </c>
-      <c r="C12" s="37" t="s">
+      <c r="C12" s="36" t="s">
         <v>288</v>
       </c>
-      <c r="D12" s="39">
+      <c r="D12" s="38">
         <v>7</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F12" s="37" t="s">
+      <c r="F12" s="36" t="s">
         <v>204</v>
       </c>
-      <c r="G12" s="37" t="s">
+      <c r="G12" s="36" t="s">
         <v>205</v>
       </c>
-      <c r="H12" s="37" t="s">
+      <c r="H12" s="36" t="s">
         <v>206</v>
       </c>
       <c r="I12" s="28">
         <v>0</v>
       </c>
-      <c r="J12" s="31">
-        <f t="shared" si="0"/>
+      <c r="J12" s="30">
+        <f>IF(I12&gt;D12,0,D12-I12)</f>
         <v>7</v>
       </c>
       <c r="K12" s="28">
-        <f t="shared" ref="K12:K57" si="3">I12+J12</f>
+        <f>I12+J12</f>
         <v>7</v>
       </c>
       <c r="L12" s="28">
-        <f t="shared" ref="L12:L62" si="4">K12-D12</f>
+        <f>K12-D12</f>
         <v>0</v>
       </c>
       <c r="M12" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D12)-L12</f>
         <v>28</v>
       </c>
       <c r="N12" s="28"/>
-      <c r="Q12" s="33" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q12" s="32" t="e">
+        <f>P12/O12</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R12" s="37" t="s">
+      <c r="R12" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="S12" s="37" t="s">
+      <c r="S12" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="37">
+      <c r="A13" s="36">
         <v>3</v>
       </c>
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="37" t="s">
         <v>289</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="36" t="s">
         <v>288</v>
       </c>
-      <c r="D13" s="39">
+      <c r="D13" s="38">
         <v>2</v>
       </c>
       <c r="E13" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F13" s="37" t="s">
+      <c r="F13" s="36" t="s">
         <v>290</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="36" t="s">
         <v>291</v>
       </c>
-      <c r="H13" s="37" t="s">
+      <c r="H13" s="36" t="s">
         <v>206</v>
       </c>
       <c r="I13" s="28">
         <v>0</v>
       </c>
-      <c r="J13" s="31">
+      <c r="J13" s="30">
         <v>10</v>
       </c>
       <c r="K13" s="28">
-        <f t="shared" si="3"/>
+        <f>I13+J13</f>
         <v>10</v>
       </c>
       <c r="L13" s="28">
-        <f t="shared" si="4"/>
+        <f>K13-D13</f>
         <v>8</v>
       </c>
       <c r="M13" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D13)-L13</f>
         <v>0</v>
       </c>
       <c r="N13" s="28"/>
-      <c r="Q13" s="33" t="e">
-        <f t="shared" si="2"/>
+      <c r="Q13" s="32" t="e">
+        <f>P13/O13</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R13" s="37" t="s">
+      <c r="R13" s="36" t="s">
         <v>285</v>
       </c>
-      <c r="S13" s="37" t="s">
+      <c r="S13" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="14" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="37">
+      <c r="A14" s="36">
         <v>4</v>
       </c>
-      <c r="B14" s="38" t="s">
+      <c r="B14" s="37" t="s">
         <v>292</v>
       </c>
-      <c r="C14" s="37" t="s">
+      <c r="C14" s="36" t="s">
         <v>293</v>
       </c>
-      <c r="D14" s="39">
+      <c r="D14" s="38">
         <v>1</v>
       </c>
       <c r="E14" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F14" s="37" t="s">
+      <c r="F14" s="36" t="s">
         <v>294</v>
       </c>
-      <c r="G14" s="37" t="s">
+      <c r="G14" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="H14" s="37" t="s">
+      <c r="H14" s="36" t="s">
         <v>206</v>
       </c>
       <c r="I14" s="28">
         <v>1</v>
       </c>
       <c r="J14" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I14&gt;D14,0,D14-I14)</f>
         <v>0</v>
       </c>
       <c r="K14" s="28">
-        <f t="shared" si="3"/>
+        <f>I14+J14</f>
         <v>1</v>
       </c>
       <c r="L14" s="28">
-        <f t="shared" si="4"/>
+        <f>K14-D14</f>
         <v>0</v>
       </c>
       <c r="M14" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D14)-L14</f>
         <v>4</v>
       </c>
       <c r="N14" s="28"/>
       <c r="O14" s="28">
         <v>430</v>
       </c>
-      <c r="Q14" s="33">
+      <c r="Q14" s="32">
         <f>P14/O14</f>
         <v>0</v>
       </c>
-      <c r="R14" s="37" t="s">
+      <c r="R14" s="36" t="s">
         <v>296</v>
       </c>
-      <c r="S14" s="37" t="s">
+      <c r="S14" s="36" t="s">
         <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="37">
+      <c r="A15" s="36">
         <v>5</v>
       </c>
-      <c r="B15" s="38" t="s">
+      <c r="B15" s="37" t="s">
         <v>298</v>
       </c>
-      <c r="C15" s="37" t="s">
+      <c r="C15" s="36" t="s">
         <v>299</v>
       </c>
-      <c r="D15" s="39">
+      <c r="D15" s="38">
         <v>6</v>
       </c>
       <c r="E15" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F15" s="37" t="s">
+      <c r="F15" s="36" t="s">
         <v>300</v>
       </c>
-      <c r="G15" s="37" t="s">
+      <c r="G15" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="H15" s="37" t="s">
+      <c r="H15" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I15" s="37">
+      <c r="I15" s="36">
         <v>4</v>
       </c>
-      <c r="J15" s="31">
-        <f t="shared" si="0"/>
+      <c r="J15" s="30">
+        <f>IF(I15&gt;D15,0,D15-I15)</f>
         <v>2</v>
       </c>
       <c r="K15" s="28">
-        <f t="shared" si="3"/>
+        <f>I15+J15</f>
         <v>6</v>
       </c>
       <c r="L15" s="28">
-        <f t="shared" si="4"/>
+        <f>K15-D15</f>
         <v>0</v>
       </c>
       <c r="M15" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D15)-L15</f>
         <v>24</v>
       </c>
       <c r="N15" s="28"/>
       <c r="O15" s="28">
         <v>100</v>
       </c>
-      <c r="P15" s="36"/>
-      <c r="Q15" s="33">
+      <c r="P15" s="35"/>
+      <c r="Q15" s="32">
         <f>P15/O15</f>
         <v>0</v>
       </c>
-      <c r="R15" s="37" t="s">
+      <c r="R15" s="36" t="s">
         <v>301</v>
       </c>
-      <c r="S15" s="37" t="s">
+      <c r="S15" s="36" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="37">
+      <c r="A16" s="36">
         <v>6</v>
       </c>
-      <c r="B16" s="38" t="s">
+      <c r="B16" s="37" t="s">
         <v>303</v>
       </c>
-      <c r="C16" s="37" t="s">
+      <c r="C16" s="36" t="s">
         <v>299</v>
       </c>
-      <c r="D16" s="39">
+      <c r="D16" s="38">
         <v>6</v>
       </c>
       <c r="E16" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="F16" s="36" t="s">
         <v>304</v>
       </c>
-      <c r="G16" s="38" t="s">
+      <c r="G16" s="37" t="s">
         <v>109</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="H16" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I16" s="37">
+      <c r="I16" s="36">
         <v>4</v>
       </c>
-      <c r="J16" s="31">
-        <f t="shared" si="0"/>
+      <c r="J16" s="30">
+        <f>IF(I16&gt;D16,0,D16-I16)</f>
         <v>2</v>
       </c>
       <c r="K16" s="28">
-        <f t="shared" si="3"/>
+        <f>I16+J16</f>
         <v>6</v>
       </c>
       <c r="L16" s="28">
-        <f t="shared" si="4"/>
+        <f>K16-D16</f>
         <v>0</v>
       </c>
       <c r="M16" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D16)-L16</f>
         <v>24</v>
       </c>
       <c r="N16" s="28"/>
       <c r="O16" s="28">
         <v>747</v>
       </c>
-      <c r="P16" s="36"/>
-      <c r="Q16" s="33">
+      <c r="P16" s="35"/>
+      <c r="Q16" s="32">
         <f>P16/O16</f>
         <v>0</v>
       </c>
-      <c r="R16" s="37" t="s">
+      <c r="R16" s="36" t="s">
         <v>305</v>
       </c>
-      <c r="S16" s="37" t="s">
+      <c r="S16" s="36" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="37">
+      <c r="A17" s="36">
         <v>7</v>
       </c>
-      <c r="B17" s="38" t="s">
+      <c r="B17" s="37" t="s">
         <v>306</v>
       </c>
-      <c r="C17" s="37" t="s">
+      <c r="C17" s="36" t="s">
         <v>307</v>
       </c>
-      <c r="D17" s="39">
+      <c r="D17" s="38">
         <v>1</v>
       </c>
       <c r="E17" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="F17" s="36" t="s">
         <v>308</v>
       </c>
-      <c r="G17" s="37" t="s">
+      <c r="G17" s="36" t="s">
         <v>30</v>
       </c>
-      <c r="H17" s="37" t="s">
+      <c r="H17" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I17" s="37">
+      <c r="I17" s="36">
         <v>1</v>
       </c>
       <c r="J17" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I17&gt;D17,0,D17-I17)</f>
         <v>0</v>
       </c>
       <c r="K17" s="28">
-        <f t="shared" si="3"/>
+        <f>I17+J17</f>
         <v>1</v>
       </c>
       <c r="L17" s="28">
-        <f t="shared" si="4"/>
+        <f>K17-D17</f>
         <v>0</v>
       </c>
       <c r="M17" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D17)-L17</f>
         <v>4</v>
       </c>
       <c r="N17" s="28"/>
-      <c r="Q17" s="33" t="e">
-        <f t="shared" ref="Q17:Q28" si="5">P17/O17</f>
+      <c r="Q17" s="32" t="e">
+        <f>P17/O17</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R17" s="37" t="s">
+      <c r="R17" s="36" t="s">
         <v>309</v>
       </c>
-      <c r="S17" s="37" t="s">
+      <c r="S17" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="18" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A18" s="37">
+      <c r="A18" s="36">
         <v>8</v>
       </c>
-      <c r="B18" s="38"/>
-      <c r="C18" s="37"/>
-      <c r="D18" s="39"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
+      <c r="B18" s="37"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="38"/>
+      <c r="F18" s="36"/>
+      <c r="G18" s="36"/>
       <c r="J18" s="28"/>
       <c r="K18" s="28"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
-      <c r="Q18" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q18" s="32" t="e">
+        <f>P18/O18</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S18" s="37" t="s">
+      <c r="S18" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="19" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A19" s="37">
+      <c r="A19" s="36">
         <v>9</v>
       </c>
-      <c r="B19" s="38"/>
-      <c r="C19" s="37"/>
-      <c r="D19" s="39"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
+      <c r="B19" s="37"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="38"/>
+      <c r="F19" s="36"/>
+      <c r="G19" s="36"/>
       <c r="J19" s="28"/>
       <c r="K19" s="28"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
-      <c r="Q19" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q19" s="32" t="e">
+        <f>P19/O19</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="S19" s="37" t="s">
+      <c r="S19" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="20" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="37">
+      <c r="A20" s="36">
         <v>10</v>
       </c>
-      <c r="B20" s="38" t="s">
+      <c r="B20" s="37" t="s">
         <v>310</v>
       </c>
-      <c r="C20" s="37" t="s">
+      <c r="C20" s="36" t="s">
         <v>311</v>
       </c>
-      <c r="D20" s="39">
+      <c r="D20" s="38">
         <v>1</v>
       </c>
       <c r="E20" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="F20" s="36" t="s">
         <v>312</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="G20" s="36" t="s">
         <v>313</v>
       </c>
-      <c r="H20" s="37" t="s">
+      <c r="H20" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I20" s="37">
+      <c r="I20" s="36">
         <v>1</v>
       </c>
       <c r="J20" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I20&gt;D20,0,D20-I20)</f>
         <v>0</v>
       </c>
       <c r="K20" s="28">
-        <f t="shared" si="3"/>
+        <f>I20+J20</f>
         <v>1</v>
       </c>
       <c r="L20" s="28">
-        <f t="shared" si="4"/>
+        <f>K20-D20</f>
         <v>0</v>
       </c>
       <c r="M20" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D20)-L20</f>
         <v>4</v>
       </c>
       <c r="N20" s="28"/>
-      <c r="Q20" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q20" s="32" t="e">
+        <f>P20/O20</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R20" s="37" t="s">
+      <c r="R20" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="S20" s="37" t="s">
+      <c r="S20" s="36" t="s">
         <v>315</v>
       </c>
-      <c r="W20" s="37" t="s">
+      <c r="W20" s="36" t="s">
         <v>316</v>
       </c>
-      <c r="Y20" s="37">
+      <c r="Y20" s="36">
         <v>8.8000000000000007</v>
       </c>
-      <c r="AB20" s="37" t="s">
+      <c r="AB20" s="36" t="s">
         <v>317</v>
       </c>
-      <c r="AC20" s="37" t="s">
+      <c r="AC20" s="36" t="s">
         <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="37">
+      <c r="A21" s="36">
         <v>11</v>
       </c>
-      <c r="B21" s="38" t="s">
+      <c r="B21" s="37" t="s">
         <v>319</v>
       </c>
-      <c r="C21" s="37" t="s">
+      <c r="C21" s="36" t="s">
         <v>320</v>
       </c>
-      <c r="D21" s="39">
+      <c r="D21" s="38">
         <v>1</v>
       </c>
       <c r="E21" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F21" s="37" t="s">
+      <c r="F21" s="36" t="s">
         <v>321</v>
       </c>
-      <c r="G21" s="37" t="s">
+      <c r="G21" s="36" t="s">
         <v>322</v>
       </c>
-      <c r="H21" s="37" t="s">
+      <c r="H21" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="I21" s="37">
+      <c r="I21" s="36">
         <v>1</v>
       </c>
       <c r="J21" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I21&gt;D21,0,D21-I21)</f>
         <v>0</v>
       </c>
       <c r="K21" s="28">
-        <f t="shared" si="3"/>
+        <f>I21+J21</f>
         <v>1</v>
       </c>
       <c r="L21" s="28">
-        <f t="shared" si="4"/>
+        <f>K21-D21</f>
         <v>0</v>
       </c>
       <c r="M21" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D21)-L21</f>
         <v>4</v>
       </c>
       <c r="N21" s="28"/>
-      <c r="Q21" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q21" s="32" t="e">
+        <f>P21/O21</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R21" s="37" t="s">
+      <c r="R21" s="36" t="s">
         <v>323</v>
       </c>
-      <c r="S21" s="37" t="s">
+      <c r="S21" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="22" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A22" s="37">
+      <c r="A22" s="36">
         <v>12</v>
       </c>
-      <c r="B22" s="38" t="s">
+      <c r="B22" s="37" t="s">
         <v>324</v>
       </c>
-      <c r="C22" s="37" t="s">
+      <c r="C22" s="36" t="s">
         <v>325</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="38">
         <v>4</v>
       </c>
       <c r="E22" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F22" s="37" t="s">
+      <c r="F22" s="36" t="s">
         <v>326</v>
       </c>
-      <c r="G22" s="37" t="s">
+      <c r="G22" s="36" t="s">
         <v>327</v>
       </c>
-      <c r="H22" s="37" t="s">
+      <c r="H22" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="I22" s="37">
+      <c r="I22" s="36">
         <v>4</v>
       </c>
       <c r="J22" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I22&gt;D22,0,D22-I22)</f>
         <v>0</v>
       </c>
       <c r="K22" s="28">
-        <f t="shared" si="3"/>
+        <f>I22+J22</f>
         <v>4</v>
       </c>
       <c r="L22" s="28">
-        <f t="shared" si="4"/>
+        <f>K22-D22</f>
         <v>0</v>
       </c>
       <c r="M22" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D22)-L22</f>
         <v>16</v>
       </c>
       <c r="N22" s="28"/>
-      <c r="Q22" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q22" s="32" t="e">
+        <f>P22/O22</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R22" s="37" t="s">
+      <c r="R22" s="36" t="s">
         <v>328</v>
       </c>
-      <c r="S22" s="37" t="s">
+      <c r="S22" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A23" s="37">
+      <c r="A23" s="36">
         <v>13</v>
       </c>
-      <c r="B23" s="38" t="s">
+      <c r="B23" s="37" t="s">
         <v>329</v>
       </c>
-      <c r="C23" s="37" t="s">
+      <c r="C23" s="36" t="s">
         <v>330</v>
       </c>
-      <c r="D23" s="39">
+      <c r="D23" s="38">
         <v>1</v>
       </c>
       <c r="E23" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F23" s="37" t="s">
+      <c r="F23" s="36" t="s">
         <v>331</v>
       </c>
-      <c r="G23" s="38" t="s">
+      <c r="G23" s="37" t="s">
         <v>332</v>
       </c>
-      <c r="H23" s="37" t="s">
+      <c r="H23" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="I23" s="37">
-        <v>0</v>
-      </c>
-      <c r="J23" s="31">
-        <f t="shared" si="0"/>
+      <c r="I23" s="36">
+        <v>0</v>
+      </c>
+      <c r="J23" s="30">
+        <f>IF(I23&gt;D23,0,D23-I23)</f>
         <v>1</v>
       </c>
       <c r="K23" s="28">
-        <f t="shared" si="3"/>
+        <f>I23+J23</f>
         <v>1</v>
       </c>
       <c r="L23" s="28">
-        <f t="shared" si="4"/>
+        <f>K23-D23</f>
         <v>0</v>
       </c>
       <c r="M23" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D23)-L23</f>
         <v>4</v>
       </c>
       <c r="N23" s="28"/>
-      <c r="Q23" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q23" s="32" t="e">
+        <f>P23/O23</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R23" s="37" t="s">
+      <c r="R23" s="36" t="s">
         <v>333</v>
       </c>
-      <c r="S23" s="37" t="s">
+      <c r="S23" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="24" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="37">
+      <c r="A24" s="36">
         <v>14</v>
       </c>
-      <c r="B24" s="38" t="s">
+      <c r="B24" s="37" t="s">
         <v>334</v>
       </c>
-      <c r="C24" s="37" t="s">
+      <c r="C24" s="36" t="s">
         <v>335</v>
       </c>
-      <c r="D24" s="39">
+      <c r="D24" s="38">
         <v>2</v>
       </c>
       <c r="E24" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F24" s="37" t="s">
+      <c r="F24" s="36" t="s">
         <v>336</v>
       </c>
-      <c r="G24" s="37" t="s">
+      <c r="G24" s="36" t="s">
         <v>337</v>
       </c>
-      <c r="H24" s="37" t="s">
+      <c r="H24" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I24" s="37">
+      <c r="I24" s="36">
         <v>2</v>
       </c>
       <c r="J24" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I24&gt;D24,0,D24-I24)</f>
         <v>0</v>
       </c>
       <c r="K24" s="28">
-        <f t="shared" si="3"/>
+        <f>I24+J24</f>
         <v>2</v>
       </c>
       <c r="L24" s="28">
-        <f t="shared" si="4"/>
+        <f>K24-D24</f>
         <v>0</v>
       </c>
       <c r="M24" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D24)-L24</f>
         <v>8</v>
       </c>
       <c r="N24" s="28"/>
-      <c r="Q24" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q24" s="32" t="e">
+        <f>P24/O24</f>
         <v>#DIV/0!</v>
       </c>
-      <c r="R24" s="37" t="s">
+      <c r="R24" s="36" t="s">
         <v>338</v>
       </c>
-      <c r="S24" s="37" t="s">
+      <c r="S24" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="25" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A25" s="37">
+      <c r="A25" s="36">
         <v>15</v>
       </c>
-      <c r="B25" s="38"/>
-      <c r="C25" s="37"/>
-      <c r="D25" s="39"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
+      <c r="B25" s="37"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="38"/>
+      <c r="F25" s="36"/>
+      <c r="G25" s="36"/>
       <c r="J25" s="28"/>
       <c r="K25" s="28"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
       <c r="N25" s="28"/>
-      <c r="Q25" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q25" s="32" t="e">
+        <f>P25/O25</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="26" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A26" s="37">
+      <c r="A26" s="36">
         <v>16</v>
       </c>
-      <c r="B26" s="38"/>
-      <c r="C26" s="37"/>
-      <c r="D26" s="39"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="37"/>
+      <c r="B26" s="37"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="38"/>
+      <c r="F26" s="36"/>
+      <c r="G26" s="36"/>
       <c r="J26" s="28"/>
       <c r="K26" s="28"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
-      <c r="Q26" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q26" s="32" t="e">
+        <f>P26/O26</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="27" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A27" s="37">
+      <c r="A27" s="36">
         <v>17</v>
       </c>
-      <c r="B27" s="38"/>
-      <c r="C27" s="37"/>
-      <c r="D27" s="39"/>
-      <c r="F27" s="37"/>
-      <c r="G27" s="37"/>
+      <c r="B27" s="37"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="38"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
       <c r="J27" s="28"/>
       <c r="K27" s="28"/>
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
       <c r="N27" s="28"/>
-      <c r="Q27" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q27" s="32" t="e">
+        <f>P27/O27</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A28" s="37">
+      <c r="A28" s="36">
         <v>18</v>
       </c>
-      <c r="B28" s="38"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="39"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="38"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
       <c r="J28" s="28"/>
       <c r="K28" s="28"/>
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
       <c r="N28" s="28"/>
-      <c r="Q28" s="33" t="e">
-        <f t="shared" si="5"/>
+      <c r="Q28" s="32" t="e">
+        <f>P28/O28</f>
         <v>#DIV/0!</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A29" s="37">
+      <c r="A29" s="36">
         <v>19</v>
       </c>
-      <c r="B29" s="38"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="39"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="36"/>
+      <c r="D29" s="38"/>
+      <c r="F29" s="36"/>
+      <c r="G29" s="36"/>
       <c r="J29" s="28"/>
       <c r="K29" s="28"/>
       <c r="L29" s="28"/>
@@ -6460,14 +6511,14 @@
       <c r="N29" s="28"/>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A30" s="37">
+      <c r="A30" s="36">
         <v>20</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="37"/>
-      <c r="D30" s="39"/>
-      <c r="F30" s="37"/>
-      <c r="G30" s="37"/>
+      <c r="B30" s="37"/>
+      <c r="C30" s="36"/>
+      <c r="D30" s="38"/>
+      <c r="F30" s="36"/>
+      <c r="G30" s="36"/>
       <c r="J30" s="28"/>
       <c r="K30" s="28"/>
       <c r="L30" s="28"/>
@@ -6475,1103 +6526,1103 @@
       <c r="N30" s="28"/>
     </row>
     <row r="31" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A31" s="37">
+      <c r="A31" s="36">
         <v>21</v>
       </c>
-      <c r="B31" s="38" t="s">
+      <c r="B31" s="37" t="s">
         <v>339</v>
       </c>
-      <c r="C31" s="37" t="s">
+      <c r="C31" s="36" t="s">
         <v>340</v>
       </c>
-      <c r="D31" s="39">
+      <c r="D31" s="38">
         <v>1</v>
       </c>
       <c r="E31" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F31" s="37" t="s">
+      <c r="F31" s="36" t="s">
         <v>341</v>
       </c>
-      <c r="G31" s="37" t="s">
+      <c r="G31" s="36" t="s">
         <v>342</v>
       </c>
-      <c r="H31" s="37" t="s">
+      <c r="H31" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I31" s="37">
+      <c r="I31" s="36">
         <v>1</v>
       </c>
       <c r="J31" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I31&gt;D31,0,D31-I31)</f>
         <v>0</v>
       </c>
       <c r="K31" s="28">
-        <f t="shared" si="3"/>
+        <f>I31+J31</f>
         <v>1</v>
       </c>
       <c r="L31" s="28">
-        <f t="shared" si="4"/>
+        <f>K31-D31</f>
         <v>0</v>
       </c>
       <c r="M31" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D31)-L31</f>
         <v>4</v>
       </c>
       <c r="N31" s="28"/>
-      <c r="R31" s="37" t="s">
+      <c r="R31" s="36" t="s">
         <v>343</v>
       </c>
-      <c r="S31" s="37" t="s">
+      <c r="S31" s="36" t="s">
         <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A32" s="37">
+      <c r="A32" s="36">
         <v>22</v>
       </c>
-      <c r="B32" s="38" t="s">
+      <c r="B32" s="37" t="s">
         <v>345</v>
       </c>
-      <c r="C32" s="37" t="s">
+      <c r="C32" s="36" t="s">
         <v>340</v>
       </c>
-      <c r="D32" s="39">
+      <c r="D32" s="38">
         <v>10</v>
       </c>
       <c r="E32" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F32" s="37" t="s">
+      <c r="F32" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="G32" s="37" t="s">
+      <c r="G32" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="H32" s="37" t="s">
+      <c r="H32" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I32" s="37">
+      <c r="I32" s="36">
         <v>2</v>
       </c>
-      <c r="J32" s="31">
+      <c r="J32" s="30">
         <v>10</v>
       </c>
       <c r="K32" s="28">
-        <f t="shared" si="3"/>
+        <f>I32+J32</f>
         <v>12</v>
       </c>
       <c r="L32" s="28">
-        <f t="shared" si="4"/>
+        <f>K32-D32</f>
         <v>2</v>
       </c>
       <c r="M32" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D32)-L32</f>
         <v>38</v>
       </c>
       <c r="N32" s="28"/>
-      <c r="R32" s="37" t="s">
+      <c r="R32" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="S32" s="37" t="s">
+      <c r="S32" s="36" t="s">
         <v>347</v>
       </c>
-      <c r="T32" s="37" t="s">
+      <c r="T32" s="36" t="s">
         <v>348</v>
       </c>
-      <c r="U32" s="37" t="s">
+      <c r="U32" s="36" t="s">
         <v>347</v>
       </c>
-      <c r="V32" s="37" t="s">
+      <c r="V32" s="36" t="s">
         <v>349</v>
       </c>
-      <c r="W32" s="37" t="s">
+      <c r="W32" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="X32" s="37" t="s">
+      <c r="X32" s="36" t="s">
         <v>350</v>
       </c>
-      <c r="Z32" s="37" t="s">
+      <c r="Z32" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="AA32" s="37" t="s">
+      <c r="AA32" s="36" t="s">
         <v>351</v>
       </c>
-      <c r="AD32" s="37" t="s">
+      <c r="AD32" s="36" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:30" ht="34" x14ac:dyDescent="0.2">
-      <c r="A33" s="37">
+      <c r="A33" s="36">
         <v>23</v>
       </c>
-      <c r="B33" s="38" t="s">
+      <c r="B33" s="37" t="s">
         <v>353</v>
       </c>
-      <c r="C33" s="37" t="s">
+      <c r="C33" s="36" t="s">
         <v>340</v>
       </c>
-      <c r="D33" s="39">
+      <c r="D33" s="38">
         <v>11</v>
       </c>
       <c r="E33" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F33" s="37" t="s">
+      <c r="F33" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G33" s="37" t="s">
+      <c r="G33" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="H33" s="37" t="s">
+      <c r="H33" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I33" s="37">
+      <c r="I33" s="36">
         <v>2</v>
       </c>
-      <c r="J33" s="31">
+      <c r="J33" s="30">
         <v>10</v>
       </c>
       <c r="K33" s="28">
-        <f t="shared" si="3"/>
+        <f>I33+J33</f>
         <v>12</v>
       </c>
       <c r="L33" s="28">
-        <f t="shared" si="4"/>
+        <f>K33-D33</f>
         <v>1</v>
       </c>
       <c r="M33" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D33)-L33</f>
         <v>43</v>
       </c>
       <c r="N33" s="28"/>
-      <c r="R33" s="37" t="s">
+      <c r="R33" s="36" t="s">
         <v>354</v>
       </c>
-      <c r="S33" s="37" t="s">
+      <c r="S33" s="36" t="s">
         <v>355</v>
       </c>
-      <c r="T33" s="37" t="s">
+      <c r="T33" s="36" t="s">
         <v>348</v>
       </c>
-      <c r="U33" s="37" t="s">
+      <c r="U33" s="36" t="s">
         <v>355</v>
       </c>
-      <c r="V33" s="37" t="s">
+      <c r="V33" s="36" t="s">
         <v>356</v>
       </c>
-      <c r="W33" s="37" t="s">
+      <c r="W33" s="36" t="s">
         <v>14</v>
       </c>
-      <c r="X33" s="37" t="s">
+      <c r="X33" s="36" t="s">
         <v>350</v>
       </c>
-      <c r="Z33" s="37" t="s">
+      <c r="Z33" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="AA33" s="37" t="s">
+      <c r="AA33" s="36" t="s">
         <v>351</v>
       </c>
-      <c r="AD33" s="37" t="s">
+      <c r="AD33" s="36" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="34" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A34" s="37">
+      <c r="A34" s="36">
         <v>24</v>
       </c>
-      <c r="B34" s="38" t="s">
+      <c r="B34" s="37" t="s">
         <v>357</v>
       </c>
-      <c r="C34" s="37" t="s">
+      <c r="C34" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D34" s="39">
+      <c r="D34" s="38">
         <v>1</v>
       </c>
       <c r="E34" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F34" s="37">
+      <c r="F34" s="36">
         <v>1E-3</v>
       </c>
-      <c r="G34" s="37"/>
-      <c r="H34" s="37" t="s">
+      <c r="G34" s="36"/>
+      <c r="H34" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I34" s="37">
+      <c r="I34" s="36">
         <v>1</v>
       </c>
       <c r="J34" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I34&gt;D34,0,D34-I34)</f>
         <v>0</v>
       </c>
       <c r="K34" s="28">
-        <f t="shared" si="3"/>
+        <f>I34+J34</f>
         <v>1</v>
       </c>
       <c r="L34" s="28">
-        <f t="shared" si="4"/>
+        <f>K34-D34</f>
         <v>0</v>
       </c>
       <c r="M34" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D34)-L34</f>
         <v>4</v>
       </c>
       <c r="N34" s="28"/>
-      <c r="R34" s="37" t="s">
+      <c r="R34" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S34" s="37" t="s">
+      <c r="S34" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="35" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A35" s="37">
+      <c r="A35" s="36">
         <v>25</v>
       </c>
-      <c r="B35" s="38" t="s">
+      <c r="B35" s="37" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D35" s="39">
+      <c r="D35" s="38">
         <v>2</v>
       </c>
       <c r="E35" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F35" s="37" t="s">
+      <c r="F35" s="36" t="s">
         <v>234</v>
       </c>
-      <c r="G35" s="37" t="s">
+      <c r="G35" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="H35" s="37" t="s">
+      <c r="H35" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I35" s="37">
-        <v>0</v>
-      </c>
-      <c r="J35" s="31">
+      <c r="I35" s="36">
+        <v>0</v>
+      </c>
+      <c r="J35" s="30">
         <v>10</v>
       </c>
       <c r="K35" s="28">
-        <f t="shared" si="3"/>
+        <f>I35+J35</f>
         <v>10</v>
       </c>
       <c r="L35" s="28">
-        <f t="shared" si="4"/>
+        <f>K35-D35</f>
         <v>8</v>
       </c>
       <c r="M35" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D35)-L35</f>
         <v>0</v>
       </c>
       <c r="N35" s="28"/>
-      <c r="R35" s="37" t="s">
+      <c r="R35" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S35" s="37" t="s">
+      <c r="S35" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="37">
+      <c r="A36" s="36">
         <v>26</v>
       </c>
-      <c r="B36" s="38" t="s">
+      <c r="B36" s="37" t="s">
         <v>361</v>
       </c>
-      <c r="C36" s="37" t="s">
+      <c r="C36" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D36" s="39">
+      <c r="D36" s="38">
         <v>1</v>
       </c>
       <c r="E36" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F36" s="37">
+      <c r="F36" s="36">
         <v>300</v>
       </c>
-      <c r="G36" s="40" t="s">
+      <c r="G36" s="39" t="s">
         <v>362</v>
       </c>
-      <c r="H36" s="37" t="s">
+      <c r="H36" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I36" s="37">
-        <v>0</v>
-      </c>
-      <c r="J36" s="41"/>
+      <c r="I36" s="36">
+        <v>0</v>
+      </c>
+      <c r="J36" s="40"/>
       <c r="K36" s="28">
-        <f t="shared" si="3"/>
+        <f>I36+J36</f>
         <v>0</v>
       </c>
       <c r="L36" s="28">
-        <f t="shared" si="4"/>
+        <f>K36-D36</f>
         <v>-1</v>
       </c>
       <c r="M36" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D36)-L36</f>
         <v>5</v>
       </c>
       <c r="N36" s="28"/>
-      <c r="R36" s="37" t="s">
+      <c r="R36" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S36" s="37" t="s">
+      <c r="S36" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="37" spans="1:30" ht="51" x14ac:dyDescent="0.2">
-      <c r="A37" s="37">
+      <c r="A37" s="36">
         <v>27</v>
       </c>
-      <c r="B37" s="38" t="s">
+      <c r="B37" s="37" t="s">
         <v>363</v>
       </c>
-      <c r="C37" s="37" t="s">
+      <c r="C37" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D37" s="39">
+      <c r="D37" s="38">
         <v>21</v>
       </c>
       <c r="E37" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F37" s="37">
+      <c r="F37" s="36">
         <v>470</v>
       </c>
-      <c r="G37" s="37" t="s">
+      <c r="G37" s="36" t="s">
         <v>364</v>
       </c>
-      <c r="H37" s="37" t="s">
+      <c r="H37" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I37" s="37">
+      <c r="I37" s="36">
         <v>11</v>
       </c>
-      <c r="J37" s="31">
+      <c r="J37" s="30">
         <v>20</v>
       </c>
       <c r="K37" s="28">
-        <f t="shared" si="3"/>
+        <f>I37+J37</f>
         <v>31</v>
       </c>
       <c r="L37" s="28">
-        <f t="shared" si="4"/>
+        <f>K37-D37</f>
         <v>10</v>
       </c>
       <c r="M37" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D37)-L37</f>
         <v>74</v>
       </c>
       <c r="N37" s="28"/>
-      <c r="R37" s="37" t="s">
+      <c r="R37" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S37" s="37" t="s">
+      <c r="S37" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A38" s="37">
+      <c r="A38" s="36">
         <v>28</v>
       </c>
-      <c r="B38" s="38" t="s">
+      <c r="B38" s="37" t="s">
         <v>365</v>
       </c>
-      <c r="C38" s="37" t="s">
+      <c r="C38" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D38" s="39">
+      <c r="D38" s="38">
         <v>6</v>
       </c>
       <c r="E38" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F38" s="37" t="s">
+      <c r="F38" s="36" t="s">
         <v>366</v>
       </c>
-      <c r="G38" s="37" t="s">
+      <c r="G38" s="36" t="s">
         <v>65</v>
       </c>
-      <c r="H38" s="37" t="s">
+      <c r="H38" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I38" s="37">
+      <c r="I38" s="36">
         <v>4</v>
       </c>
-      <c r="J38" s="31">
+      <c r="J38" s="30">
         <v>10</v>
       </c>
       <c r="K38" s="28">
-        <f t="shared" si="3"/>
+        <f>I38+J38</f>
         <v>14</v>
       </c>
       <c r="L38" s="28">
-        <f t="shared" si="4"/>
+        <f>K38-D38</f>
         <v>8</v>
       </c>
       <c r="M38" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D38)-L38</f>
         <v>16</v>
       </c>
       <c r="N38" s="28"/>
-      <c r="R38" s="37" t="s">
+      <c r="R38" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S38" s="37" t="s">
+      <c r="S38" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="39" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A39" s="37">
+      <c r="A39" s="36">
         <v>29</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="37" t="s">
         <v>367</v>
       </c>
-      <c r="C39" s="37" t="s">
+      <c r="C39" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D39" s="39">
+      <c r="D39" s="38">
         <v>3</v>
       </c>
       <c r="E39" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F39" s="37" t="s">
+      <c r="F39" s="36" t="s">
         <v>368</v>
       </c>
-      <c r="G39" s="37" t="s">
+      <c r="G39" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="H39" s="37" t="s">
+      <c r="H39" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I39" s="37">
+      <c r="I39" s="36">
         <v>8</v>
       </c>
       <c r="J39" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I39&gt;D39,0,D39-I39)</f>
         <v>0</v>
       </c>
       <c r="K39" s="28">
-        <f t="shared" si="3"/>
+        <f>I39+J39</f>
         <v>8</v>
       </c>
       <c r="L39" s="28">
-        <f t="shared" si="4"/>
+        <f>K39-D39</f>
         <v>5</v>
       </c>
       <c r="M39" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D39)-L39</f>
         <v>7</v>
       </c>
       <c r="N39" s="28"/>
-      <c r="R39" s="37" t="s">
+      <c r="R39" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S39" s="37" t="s">
+      <c r="S39" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="40" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A40" s="37">
+      <c r="A40" s="36">
         <v>30</v>
       </c>
-      <c r="B40" s="38" t="s">
+      <c r="B40" s="37" t="s">
         <v>369</v>
       </c>
-      <c r="C40" s="37" t="s">
+      <c r="C40" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D40" s="39">
+      <c r="D40" s="38">
         <v>2</v>
       </c>
       <c r="E40" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F40" s="37" t="s">
+      <c r="F40" s="36" t="s">
         <v>370</v>
       </c>
-      <c r="G40" s="37" t="s">
+      <c r="G40" s="36" t="s">
         <v>94</v>
       </c>
-      <c r="H40" s="37" t="s">
+      <c r="H40" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I40" s="37">
+      <c r="I40" s="36">
         <v>8</v>
       </c>
       <c r="J40" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I40&gt;D40,0,D40-I40)</f>
         <v>0</v>
       </c>
       <c r="K40" s="28">
-        <f t="shared" si="3"/>
+        <f>I40+J40</f>
         <v>8</v>
       </c>
       <c r="L40" s="28">
-        <f t="shared" si="4"/>
+        <f>K40-D40</f>
         <v>6</v>
       </c>
       <c r="M40" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D40)-L40</f>
         <v>2</v>
       </c>
       <c r="N40" s="28"/>
-      <c r="R40" s="37" t="s">
+      <c r="R40" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S40" s="37" t="s">
+      <c r="S40" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="41" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A41" s="37">
+      <c r="A41" s="36">
         <v>31</v>
       </c>
-      <c r="B41" s="38" t="s">
+      <c r="B41" s="37" t="s">
         <v>371</v>
       </c>
-      <c r="C41" s="37" t="s">
+      <c r="C41" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D41" s="39">
+      <c r="D41" s="38">
         <v>2</v>
       </c>
       <c r="E41" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F41" s="37">
+      <c r="F41" s="36">
         <v>11</v>
       </c>
-      <c r="G41" s="37" t="s">
+      <c r="G41" s="36" t="s">
         <v>372</v>
       </c>
-      <c r="H41" s="37" t="s">
+      <c r="H41" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I41" s="37">
-        <v>0</v>
-      </c>
-      <c r="J41" s="31">
+      <c r="I41" s="36">
+        <v>0</v>
+      </c>
+      <c r="J41" s="30">
         <v>10</v>
       </c>
       <c r="K41" s="28">
-        <f t="shared" si="3"/>
+        <f>I41+J41</f>
         <v>10</v>
       </c>
       <c r="L41" s="28">
-        <f t="shared" si="4"/>
+        <f>K41-D41</f>
         <v>8</v>
       </c>
       <c r="M41" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D41)-L41</f>
         <v>0</v>
       </c>
       <c r="N41" s="28"/>
-      <c r="R41" s="37" t="s">
+      <c r="R41" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S41" s="37" t="s">
+      <c r="S41" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A42" s="37">
+      <c r="A42" s="36">
         <v>32</v>
       </c>
-      <c r="B42" s="38" t="s">
+      <c r="B42" s="37" t="s">
         <v>373</v>
       </c>
-      <c r="C42" s="37" t="s">
+      <c r="C42" s="36" t="s">
         <v>358</v>
       </c>
-      <c r="D42" s="39">
+      <c r="D42" s="38">
         <v>6</v>
       </c>
       <c r="E42" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F42" s="37" t="s">
+      <c r="F42" s="36" t="s">
         <v>374</v>
       </c>
-      <c r="G42" s="37" t="s">
+      <c r="G42" s="36" t="s">
         <v>82</v>
       </c>
-      <c r="H42" s="37" t="s">
+      <c r="H42" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I42" s="37">
+      <c r="I42" s="36">
         <v>6</v>
       </c>
       <c r="J42" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I42&gt;D42,0,D42-I42)</f>
         <v>0</v>
       </c>
       <c r="K42" s="28">
-        <f t="shared" si="3"/>
+        <f>I42+J42</f>
         <v>6</v>
       </c>
       <c r="L42" s="28">
-        <f t="shared" si="4"/>
+        <f>K42-D42</f>
         <v>0</v>
       </c>
       <c r="M42" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D42)-L42</f>
         <v>24</v>
       </c>
       <c r="N42" s="28"/>
-      <c r="R42" s="37" t="s">
+      <c r="R42" s="36" t="s">
         <v>359</v>
       </c>
-      <c r="S42" s="37" t="s">
+      <c r="S42" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="43" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A43" s="37">
+      <c r="A43" s="36">
         <v>33</v>
       </c>
-      <c r="B43" s="38" t="s">
+      <c r="B43" s="37" t="s">
         <v>375</v>
       </c>
-      <c r="C43" s="37" t="s">
+      <c r="C43" s="36" t="s">
         <v>376</v>
       </c>
-      <c r="D43" s="39">
+      <c r="D43" s="38">
         <v>1</v>
       </c>
       <c r="E43" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F43" s="37" t="s">
+      <c r="F43" s="36" t="s">
         <v>377</v>
       </c>
-      <c r="G43" s="37" t="s">
+      <c r="G43" s="36" t="s">
         <v>378</v>
       </c>
-      <c r="H43" s="37" t="s">
+      <c r="H43" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I43" s="37">
+      <c r="I43" s="36">
         <v>1</v>
       </c>
       <c r="J43" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I43&gt;D43,0,D43-I43)</f>
         <v>0</v>
       </c>
       <c r="K43" s="28">
-        <f t="shared" si="3"/>
+        <f>I43+J43</f>
         <v>1</v>
       </c>
       <c r="L43" s="28">
-        <f t="shared" si="4"/>
+        <f>K43-D43</f>
         <v>0</v>
       </c>
       <c r="M43" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D43)-L43</f>
         <v>4</v>
       </c>
       <c r="N43" s="28"/>
-      <c r="R43" s="37" t="s">
+      <c r="R43" s="36" t="s">
         <v>379</v>
       </c>
-      <c r="S43" s="37" t="s">
+      <c r="S43" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="44" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A44" s="37">
+      <c r="A44" s="36">
         <v>34</v>
       </c>
-      <c r="B44" s="38" t="s">
+      <c r="B44" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="C44" s="37" t="s">
+      <c r="C44" s="36" t="s">
         <v>380</v>
       </c>
-      <c r="D44" s="39">
+      <c r="D44" s="38">
         <v>1</v>
       </c>
       <c r="E44" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F44" s="37" t="s">
+      <c r="F44" s="36" t="s">
         <v>381</v>
       </c>
-      <c r="G44" s="37" t="s">
+      <c r="G44" s="36" t="s">
         <v>382</v>
       </c>
-      <c r="H44" s="37" t="s">
+      <c r="H44" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I44" s="37">
+      <c r="I44" s="36">
         <v>1</v>
       </c>
       <c r="J44" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I44&gt;D44,0,D44-I44)</f>
         <v>0</v>
       </c>
       <c r="K44" s="28">
-        <f t="shared" si="3"/>
+        <f>I44+J44</f>
         <v>1</v>
       </c>
       <c r="L44" s="28">
-        <f t="shared" si="4"/>
+        <f>K44-D44</f>
         <v>0</v>
       </c>
       <c r="M44" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D44)-L44</f>
         <v>4</v>
       </c>
       <c r="N44" s="28"/>
-      <c r="R44" s="37" t="s">
+      <c r="R44" s="36" t="s">
         <v>383</v>
       </c>
-      <c r="S44" s="37" t="s">
+      <c r="S44" s="36" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="45" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A45" s="37">
+      <c r="A45" s="36">
         <v>35</v>
       </c>
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="37" t="s">
         <v>385</v>
       </c>
-      <c r="C45" s="37" t="s">
+      <c r="C45" s="36" t="s">
         <v>386</v>
       </c>
-      <c r="D45" s="39">
+      <c r="D45" s="38">
         <v>1</v>
       </c>
       <c r="E45" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F45" s="37" t="s">
+      <c r="F45" s="36" t="s">
         <v>137</v>
       </c>
-      <c r="G45" s="37"/>
-      <c r="H45" s="37" t="s">
+      <c r="G45" s="36"/>
+      <c r="H45" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I45" s="37">
+      <c r="I45" s="36">
         <v>2</v>
       </c>
       <c r="J45" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I45&gt;D45,0,D45-I45)</f>
         <v>0</v>
       </c>
       <c r="K45" s="28">
-        <f t="shared" si="3"/>
+        <f>I45+J45</f>
         <v>2</v>
       </c>
       <c r="L45" s="28">
-        <f t="shared" si="4"/>
+        <f>K45-D45</f>
         <v>1</v>
       </c>
       <c r="M45" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D45)-L45</f>
         <v>3</v>
       </c>
       <c r="N45" s="28"/>
-      <c r="R45" s="37" t="s">
+      <c r="R45" s="36" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="46" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A46" s="37">
+      <c r="A46" s="36">
         <v>36</v>
       </c>
-      <c r="B46" s="38" t="s">
+      <c r="B46" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="C46" s="37" t="s">
+      <c r="C46" s="36" t="s">
         <v>388</v>
       </c>
-      <c r="D46" s="39">
+      <c r="D46" s="38">
         <v>1</v>
       </c>
       <c r="E46" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F46" s="37" t="s">
+      <c r="F46" s="36" t="s">
         <v>389</v>
       </c>
-      <c r="G46" s="37" t="s">
+      <c r="G46" s="36" t="s">
         <v>390</v>
       </c>
-      <c r="H46" s="37" t="s">
+      <c r="H46" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I46" s="37">
-        <v>0</v>
-      </c>
-      <c r="J46" s="31">
-        <f t="shared" si="0"/>
+      <c r="I46" s="36">
+        <v>0</v>
+      </c>
+      <c r="J46" s="30">
+        <f>IF(I46&gt;D46,0,D46-I46)</f>
         <v>1</v>
       </c>
       <c r="K46" s="28">
-        <f t="shared" si="3"/>
+        <f>I46+J46</f>
         <v>1</v>
       </c>
       <c r="L46" s="28">
-        <f t="shared" si="4"/>
+        <f>K46-D46</f>
         <v>0</v>
       </c>
       <c r="M46" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D46)-L46</f>
         <v>4</v>
       </c>
       <c r="N46" s="28"/>
-      <c r="R46" s="37" t="s">
+      <c r="R46" s="36" t="s">
         <v>391</v>
       </c>
-      <c r="S46" s="37" t="s">
+      <c r="S46" s="36" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="47" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A47" s="37">
+      <c r="A47" s="36">
         <v>37</v>
       </c>
-      <c r="B47" s="38" t="s">
+      <c r="B47" s="37" t="s">
         <v>393</v>
       </c>
-      <c r="C47" s="37" t="s">
+      <c r="C47" s="36" t="s">
         <v>394</v>
       </c>
-      <c r="D47" s="39">
+      <c r="D47" s="38">
         <v>1</v>
       </c>
       <c r="E47" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F47" s="37" t="s">
+      <c r="F47" s="36" t="s">
         <v>395</v>
       </c>
-      <c r="G47" s="37" t="s">
+      <c r="G47" s="36" t="s">
         <v>396</v>
       </c>
-      <c r="H47" s="37" t="s">
+      <c r="H47" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I47" s="37">
+      <c r="I47" s="36">
         <v>1</v>
       </c>
       <c r="J47" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I47&gt;D47,0,D47-I47)</f>
         <v>0</v>
       </c>
       <c r="K47" s="28">
-        <f t="shared" si="3"/>
+        <f>I47+J47</f>
         <v>1</v>
       </c>
       <c r="L47" s="28">
-        <f t="shared" si="4"/>
+        <f>K47-D47</f>
         <v>0</v>
       </c>
       <c r="M47" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D47)-L47</f>
         <v>4</v>
       </c>
       <c r="N47" s="28"/>
-      <c r="R47" s="37" t="s">
+      <c r="R47" s="36" t="s">
         <v>397</v>
       </c>
-      <c r="S47" s="37" t="s">
+      <c r="S47" s="36" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="48" spans="1:30" ht="17" x14ac:dyDescent="0.2">
-      <c r="A48" s="37">
+      <c r="A48" s="36">
         <v>38</v>
       </c>
-      <c r="B48" s="38" t="s">
+      <c r="B48" s="37" t="s">
         <v>399</v>
       </c>
-      <c r="C48" s="37" t="s">
+      <c r="C48" s="36" t="s">
         <v>400</v>
       </c>
-      <c r="D48" s="39">
+      <c r="D48" s="38">
         <v>2</v>
       </c>
       <c r="E48" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F48" s="37" t="s">
+      <c r="F48" s="36" t="s">
         <v>401</v>
       </c>
-      <c r="G48" s="37" t="s">
+      <c r="G48" s="36" t="s">
         <v>402</v>
       </c>
-      <c r="H48" s="37" t="s">
+      <c r="H48" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I48" s="37">
+      <c r="I48" s="36">
         <v>2</v>
       </c>
       <c r="J48" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I48&gt;D48,0,D48-I48)</f>
         <v>0</v>
       </c>
       <c r="K48" s="28">
-        <f t="shared" si="3"/>
+        <f>I48+J48</f>
         <v>2</v>
       </c>
       <c r="L48" s="28">
-        <f t="shared" si="4"/>
+        <f>K48-D48</f>
         <v>0</v>
       </c>
       <c r="M48" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D48)-L48</f>
         <v>8</v>
       </c>
       <c r="N48" s="28"/>
-      <c r="R48" s="37" t="s">
+      <c r="R48" s="36" t="s">
         <v>403</v>
       </c>
-      <c r="S48" s="37" t="s">
+      <c r="S48" s="36" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A49" s="37">
+      <c r="A49" s="36">
         <v>39</v>
       </c>
-      <c r="B49" s="38" t="s">
+      <c r="B49" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="C49" s="37" t="s">
+      <c r="C49" s="36" t="s">
         <v>405</v>
       </c>
-      <c r="D49" s="39">
+      <c r="D49" s="38">
         <v>1</v>
       </c>
       <c r="E49" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F49" s="37" t="s">
+      <c r="F49" s="36" t="s">
         <v>406</v>
       </c>
-      <c r="G49" s="37" t="s">
+      <c r="G49" s="36" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="37" t="s">
+      <c r="H49" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I49" s="37">
+      <c r="I49" s="36">
         <v>1</v>
       </c>
       <c r="J49" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I49&gt;D49,0,D49-I49)</f>
         <v>0</v>
       </c>
       <c r="K49" s="28">
-        <f t="shared" si="3"/>
+        <f>I49+J49</f>
         <v>1</v>
       </c>
       <c r="L49" s="28">
-        <f t="shared" si="4"/>
+        <f>K49-D49</f>
         <v>0</v>
       </c>
       <c r="M49" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D49)-L49</f>
         <v>4</v>
       </c>
       <c r="N49" s="28"/>
-      <c r="R49" s="37" t="s">
+      <c r="R49" s="36" t="s">
         <v>407</v>
       </c>
-      <c r="S49" s="37" t="s">
+      <c r="S49" s="36" t="s">
         <v>408</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A50" s="37">
+      <c r="A50" s="36">
         <v>40</v>
       </c>
-      <c r="B50" s="38" t="s">
+      <c r="B50" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="C50" s="37" t="s">
+      <c r="C50" s="36" t="s">
         <v>409</v>
       </c>
-      <c r="D50" s="39">
+      <c r="D50" s="38">
         <v>1</v>
       </c>
       <c r="E50" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F50" s="37" t="s">
+      <c r="F50" s="36" t="s">
         <v>410</v>
       </c>
-      <c r="G50" s="37" t="s">
+      <c r="G50" s="36" t="s">
         <v>411</v>
       </c>
-      <c r="H50" s="37" t="s">
+      <c r="H50" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I50" s="37">
+      <c r="I50" s="36">
         <v>1</v>
       </c>
       <c r="J50" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I50&gt;D50,0,D50-I50)</f>
         <v>0</v>
       </c>
       <c r="K50" s="28">
-        <f t="shared" si="3"/>
+        <f>I50+J50</f>
         <v>1</v>
       </c>
       <c r="L50" s="28">
-        <f t="shared" si="4"/>
+        <f>K50-D50</f>
         <v>0</v>
       </c>
       <c r="M50" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D50)-L50</f>
         <v>4</v>
       </c>
       <c r="N50" s="28"/>
-      <c r="R50" s="37" t="s">
+      <c r="R50" s="36" t="s">
         <v>412</v>
       </c>
-      <c r="S50" s="37" t="s">
+      <c r="S50" s="36" t="s">
         <v>413</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A51" s="37">
+      <c r="A51" s="36">
         <v>41</v>
       </c>
-      <c r="B51" s="38" t="s">
+      <c r="B51" s="37" t="s">
         <v>251</v>
       </c>
-      <c r="C51" s="37" t="s">
+      <c r="C51" s="36" t="s">
         <v>414</v>
       </c>
-      <c r="D51" s="39">
+      <c r="D51" s="38">
         <v>1</v>
       </c>
       <c r="E51" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F51" s="37" t="s">
+      <c r="F51" s="36" t="s">
         <v>415</v>
       </c>
-      <c r="G51" s="38" t="s">
+      <c r="G51" s="37" t="s">
         <v>416</v>
       </c>
-      <c r="H51" s="37" t="s">
+      <c r="H51" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="I51" s="37">
+      <c r="I51" s="36">
         <v>1</v>
       </c>
       <c r="J51" s="28">
@@ -7583,432 +7634,390 @@
         <v>1</v>
       </c>
       <c r="L51" s="28">
-        <f t="shared" si="4"/>
+        <f>K51-D51</f>
         <v>0</v>
       </c>
       <c r="M51" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D51)-L51</f>
         <v>4</v>
       </c>
       <c r="N51" s="28"/>
-      <c r="R51" s="37" t="s">
+      <c r="R51" s="36" t="s">
         <v>417</v>
       </c>
-      <c r="S51" s="37" t="s">
+      <c r="S51" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A52" s="37">
+      <c r="A52" s="36">
         <v>42</v>
       </c>
-      <c r="B52" s="38" t="s">
+      <c r="B52" s="37" t="s">
         <v>418</v>
       </c>
-      <c r="C52" s="37" t="s">
+      <c r="C52" s="36" t="s">
         <v>419</v>
       </c>
-      <c r="D52" s="39">
+      <c r="D52" s="38">
         <v>1</v>
       </c>
       <c r="E52" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F52" s="37" t="s">
+      <c r="F52" s="36" t="s">
         <v>420</v>
       </c>
-      <c r="G52" s="37" t="s">
+      <c r="G52" s="36" t="s">
         <v>421</v>
       </c>
-      <c r="H52" s="37" t="s">
+      <c r="H52" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="I52" s="37">
+      <c r="I52" s="36">
         <v>1</v>
       </c>
       <c r="J52" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I52&gt;D52,0,D52-I52)</f>
         <v>0</v>
       </c>
       <c r="K52" s="28">
-        <f t="shared" si="3"/>
+        <f>I52+J52</f>
         <v>1</v>
       </c>
       <c r="L52" s="28">
-        <f t="shared" si="4"/>
+        <f>K52-D52</f>
         <v>0</v>
       </c>
       <c r="M52" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D52)-L52</f>
         <v>4</v>
       </c>
       <c r="N52" s="28"/>
-      <c r="R52" s="37" t="s">
+      <c r="R52" s="36" t="s">
         <v>422</v>
       </c>
-      <c r="S52" s="37" t="s">
+      <c r="S52" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="53" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A53" s="37">
+      <c r="A53" s="36">
         <v>43</v>
       </c>
-      <c r="B53" s="38" t="s">
+      <c r="B53" s="37" t="s">
         <v>423</v>
       </c>
-      <c r="C53" s="37" t="s">
+      <c r="C53" s="36" t="s">
         <v>424</v>
       </c>
-      <c r="D53" s="39">
+      <c r="D53" s="38">
         <v>1</v>
       </c>
       <c r="E53" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F53" s="37" t="s">
+      <c r="F53" s="36" t="s">
         <v>425</v>
       </c>
-      <c r="G53" s="37"/>
-      <c r="H53" s="37" t="s">
+      <c r="G53" s="36"/>
+      <c r="H53" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="I53" s="37">
+      <c r="I53" s="36">
         <v>1</v>
       </c>
       <c r="J53" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I53&gt;D53,0,D53-I53)</f>
         <v>0</v>
       </c>
       <c r="K53" s="28">
-        <f t="shared" si="3"/>
+        <f>I53+J53</f>
         <v>1</v>
       </c>
       <c r="L53" s="28">
-        <f t="shared" si="4"/>
+        <f>K53-D53</f>
         <v>0</v>
       </c>
       <c r="M53" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D53)-L53</f>
         <v>4</v>
       </c>
       <c r="N53" s="28"/>
-      <c r="R53" s="37" t="s">
+      <c r="R53" s="36" t="s">
         <v>426</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A54" s="37">
+      <c r="A54" s="36">
         <v>101</v>
       </c>
-      <c r="D54" s="39">
-        <v>1</v>
-      </c>
-      <c r="F54" s="37" t="s">
+      <c r="D54" s="38">
+        <v>1</v>
+      </c>
+      <c r="F54" s="36" t="s">
         <v>427</v>
       </c>
-      <c r="G54" s="37" t="s">
+      <c r="G54" s="36" t="s">
         <v>428</v>
       </c>
-      <c r="H54" s="37" t="s">
+      <c r="H54" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="I54" s="37">
-        <v>0</v>
-      </c>
-      <c r="J54" s="31">
-        <f t="shared" si="0"/>
+      <c r="I54" s="36">
+        <v>0</v>
+      </c>
+      <c r="J54" s="30">
+        <f>IF(I54&gt;D54,0,D54-I54)</f>
         <v>1</v>
       </c>
       <c r="K54" s="28">
-        <f t="shared" si="3"/>
+        <f>I54+J54</f>
         <v>1</v>
       </c>
       <c r="L54" s="28">
-        <f t="shared" si="4"/>
+        <f>K54-D54</f>
         <v>0</v>
       </c>
       <c r="M54" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D54)-L54</f>
         <v>4</v>
       </c>
       <c r="N54" s="28"/>
     </row>
     <row r="55" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A55" s="37">
+      <c r="A55" s="36">
         <v>102</v>
       </c>
-      <c r="B55" s="38" t="s">
+      <c r="B55" s="37" t="s">
         <v>281</v>
       </c>
-      <c r="C55" s="37" t="s">
+      <c r="C55" s="36" t="s">
         <v>282</v>
       </c>
-      <c r="D55" s="39">
+      <c r="D55" s="38">
         <v>2</v>
       </c>
       <c r="E55" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F55" s="37" t="s">
+      <c r="F55" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="G55" s="38" t="s">
+      <c r="G55" s="37" t="s">
         <v>430</v>
       </c>
-      <c r="H55" s="37" t="s">
+      <c r="H55" s="36" t="s">
         <v>229</v>
       </c>
-      <c r="I55" s="37">
-        <v>0</v>
-      </c>
-      <c r="J55" s="31">
-        <f t="shared" si="0"/>
+      <c r="I55" s="36">
+        <v>0</v>
+      </c>
+      <c r="J55" s="30">
+        <f>IF(I55&gt;D55,0,D55-I55)</f>
         <v>2</v>
       </c>
       <c r="K55" s="28">
-        <f t="shared" si="3"/>
+        <f>I55+J55</f>
         <v>2</v>
       </c>
       <c r="L55" s="28">
-        <f t="shared" si="4"/>
+        <f>K55-D55</f>
         <v>0</v>
       </c>
       <c r="M55" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D55)-L55</f>
         <v>8</v>
       </c>
       <c r="N55" s="28"/>
     </row>
     <row r="56" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A56" s="37">
+      <c r="A56" s="36">
         <v>103</v>
       </c>
-      <c r="B56" s="38" t="s">
+      <c r="B56" s="37" t="s">
         <v>431</v>
       </c>
-      <c r="C56" s="37" t="s">
+      <c r="C56" s="36" t="s">
         <v>335</v>
       </c>
-      <c r="D56" s="39">
+      <c r="D56" s="38">
         <v>2</v>
       </c>
       <c r="E56" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F56" s="37" t="s">
+      <c r="F56" s="36" t="s">
         <v>336</v>
       </c>
-      <c r="G56" s="37" t="s">
+      <c r="G56" s="36" t="s">
         <v>337</v>
       </c>
-      <c r="H56" s="37" t="s">
+      <c r="H56" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I56" s="37">
+      <c r="I56" s="36">
         <v>2</v>
       </c>
       <c r="J56" s="28">
-        <f t="shared" si="0"/>
+        <f>IF(I56&gt;D56,0,D56-I56)</f>
         <v>0</v>
       </c>
       <c r="K56" s="28">
-        <f t="shared" si="3"/>
+        <f>I56+J56</f>
         <v>2</v>
       </c>
       <c r="L56" s="28">
-        <f t="shared" si="4"/>
+        <f>K56-D56</f>
         <v>0</v>
       </c>
       <c r="M56" s="28">
-        <f t="shared" si="1"/>
+        <f>(4*D56)-L56</f>
         <v>8</v>
       </c>
       <c r="N56" s="28"/>
-      <c r="R56" s="37" t="s">
+      <c r="R56" s="36" t="s">
         <v>338</v>
       </c>
-      <c r="S56" s="37" t="s">
+      <c r="S56" s="36" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="57" spans="1:19" ht="34" x14ac:dyDescent="0.2">
-      <c r="A57" s="37">
+      <c r="A57" s="36">
         <v>104</v>
       </c>
-      <c r="B57" s="37" t="s">
+      <c r="B57" s="36" t="s">
         <v>431</v>
       </c>
-      <c r="C57" s="38" t="s">
+      <c r="C57" s="37" t="s">
         <v>432</v>
       </c>
-      <c r="D57" s="39">
+      <c r="D57" s="38">
         <v>1</v>
       </c>
       <c r="E57" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F57" s="38" t="s">
+      <c r="F57" s="37" t="s">
         <v>433</v>
       </c>
-      <c r="G57" s="38" t="s">
+      <c r="G57" s="37" t="s">
         <v>434</v>
       </c>
-      <c r="H57" s="37" t="s">
+      <c r="H57" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I57" s="37">
-        <v>1</v>
-      </c>
-      <c r="J57" s="37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K57" s="37">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="L57" s="37">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M57" s="37">
-        <f t="shared" si="1"/>
+      <c r="I57" s="36">
+        <v>1</v>
+      </c>
+      <c r="J57" s="36">
+        <f>IF(I57&gt;D57,0,D57-I57)</f>
+        <v>0</v>
+      </c>
+      <c r="K57" s="36">
+        <f>I57+J57</f>
+        <v>1</v>
+      </c>
+      <c r="L57" s="36">
+        <f>K57-D57</f>
+        <v>0</v>
+      </c>
+      <c r="M57" s="36">
+        <f>(4*D57)-L57</f>
         <v>4</v>
       </c>
     </row>
     <row r="58" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A58" s="37">
+      <c r="A58" s="36">
         <v>105</v>
       </c>
-      <c r="B58" s="37" t="s">
+      <c r="B58" s="36" t="s">
         <v>142</v>
       </c>
-      <c r="D58" s="39">
+      <c r="D58" s="38">
         <v>1</v>
       </c>
       <c r="E58" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="G58" s="38" t="s">
+      <c r="G58" s="37" t="s">
         <v>435</v>
       </c>
-      <c r="H58" s="37" t="s">
+      <c r="H58" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I58" s="37">
+      <c r="I58" s="36">
         <v>5</v>
       </c>
-      <c r="J58" s="37">
+      <c r="J58" s="36">
         <f>IF(I58&gt;D58,0,D58-I58)</f>
         <v>0</v>
       </c>
-      <c r="K58" s="37">
+      <c r="K58" s="36">
         <f>I58+J58</f>
         <v>5</v>
       </c>
-      <c r="L58" s="37">
-        <f t="shared" si="4"/>
+      <c r="L58" s="36">
+        <f>K58-D58</f>
         <v>4</v>
       </c>
-      <c r="M58" s="37">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:19" ht="17" x14ac:dyDescent="0.2">
-      <c r="A59" s="37">
-        <v>106</v>
-      </c>
-      <c r="B59" s="37" t="s">
-        <v>436</v>
-      </c>
-      <c r="C59" s="38" t="s">
-        <v>437</v>
-      </c>
-      <c r="D59" s="39">
-        <v>1</v>
-      </c>
-      <c r="E59" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="G59" s="38" t="s">
-        <v>438</v>
-      </c>
-      <c r="H59" s="37" t="s">
-        <v>206</v>
-      </c>
-      <c r="I59" s="37">
-        <v>1</v>
-      </c>
-      <c r="J59" s="37">
-        <f t="shared" ref="J59:J62" si="6">IF(I59&gt;D59,0,D59-I59)</f>
-        <v>0</v>
-      </c>
-      <c r="K59" s="37">
-        <f t="shared" ref="K59:K62" si="7">I59+J59</f>
-        <v>1</v>
-      </c>
-      <c r="L59" s="37">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M59" s="37">
-        <f t="shared" si="1"/>
-        <v>4</v>
+      <c r="M58" s="36">
+        <f>(4*D58)-L58</f>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J60" s="37">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K60" s="37">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L60" s="37">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M60" s="37">
-        <f t="shared" si="1"/>
+      <c r="J60" s="36">
+        <f>IF(I60&gt;D60,0,D60-I60)</f>
+        <v>0</v>
+      </c>
+      <c r="K60" s="36">
+        <f>I60+J60</f>
+        <v>0</v>
+      </c>
+      <c r="L60" s="36">
+        <f>K60-D60</f>
+        <v>0</v>
+      </c>
+      <c r="M60" s="36">
+        <f>(4*D60)-L60</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J61" s="37">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K61" s="37">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L61" s="37">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M61" s="37">
-        <f t="shared" si="1"/>
+      <c r="J61" s="36">
+        <f>IF(I61&gt;D61,0,D61-I61)</f>
+        <v>0</v>
+      </c>
+      <c r="K61" s="36">
+        <f>I61+J61</f>
+        <v>0</v>
+      </c>
+      <c r="L61" s="36">
+        <f>K61-D61</f>
+        <v>0</v>
+      </c>
+      <c r="M61" s="36">
+        <f>(4*D61)-L61</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="J62" s="37">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K62" s="37">
-        <f t="shared" si="7"/>
-        <v>0</v>
-      </c>
-      <c r="L62" s="37">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M62" s="37">
-        <f t="shared" si="1"/>
+      <c r="J62" s="36">
+        <f>IF(I62&gt;D62,0,D62-I62)</f>
+        <v>0</v>
+      </c>
+      <c r="K62" s="36">
+        <f>I62+J62</f>
+        <v>0</v>
+      </c>
+      <c r="L62" s="36">
+        <f>K62-D62</f>
+        <v>0</v>
+      </c>
+      <c r="M62" s="36">
+        <f>(4*D62)-L62</f>
         <v>0</v>
       </c>
     </row>
@@ -8018,4 +8027,463 @@
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87AFCDAF-E620-294C-BC98-AFD17B703801}">
+  <dimension ref="A1:Q31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="10.83203125" style="28"/>
+    <col min="2" max="2" width="17" style="28" customWidth="1"/>
+    <col min="3" max="3" width="39.6640625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.83203125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="22.83203125" style="28" customWidth="1"/>
+    <col min="7" max="7" width="28.5" style="28" customWidth="1"/>
+    <col min="8" max="8" width="9.6640625" style="28" customWidth="1"/>
+    <col min="9" max="9" width="28" style="28" customWidth="1"/>
+    <col min="10" max="11" width="18.5" style="28" customWidth="1"/>
+    <col min="12" max="12" width="28.33203125" style="28" customWidth="1"/>
+    <col min="13" max="13" width="16.33203125" style="28" customWidth="1"/>
+    <col min="14" max="14" width="5.83203125" style="28" customWidth="1"/>
+    <col min="15" max="15" width="16.33203125" style="28" customWidth="1"/>
+    <col min="16" max="16" width="10.83203125" style="28"/>
+    <col min="17" max="17" width="9.1640625" style="28" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="28"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A1" s="27" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A2" s="27" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.15">
+      <c r="A3" s="29">
+        <v>43970</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>173</v>
+      </c>
+      <c r="O3" s="42" t="s">
+        <v>174</v>
+      </c>
+      <c r="P3" s="42"/>
+      <c r="Q3" s="42"/>
+    </row>
+    <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
+      <c r="A4" s="29"/>
+      <c r="B4" s="27"/>
+      <c r="J4" s="30" t="s">
+        <v>175</v>
+      </c>
+      <c r="K4" s="30" t="s">
+        <v>176</v>
+      </c>
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+    </row>
+    <row r="5" spans="1:17" ht="34" x14ac:dyDescent="0.15">
+      <c r="B5" s="30" t="s">
+        <v>177</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>178</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>179</v>
+      </c>
+      <c r="I5" s="28" t="s">
+        <v>180</v>
+      </c>
+      <c r="J5" s="41" t="s">
+        <v>181</v>
+      </c>
+      <c r="K5" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="L5" s="28" t="s">
+        <v>183</v>
+      </c>
+      <c r="M5" s="28" t="s">
+        <v>184</v>
+      </c>
+      <c r="O5" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="P5" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q5" s="28" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17" x14ac:dyDescent="0.15">
+      <c r="A6" s="28" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="28" t="s">
+        <v>189</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>190</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>148</v>
+      </c>
+      <c r="E6" s="28" t="s">
+        <v>191</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>268</v>
+      </c>
+      <c r="G6" s="28" t="s">
+        <v>192</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>193</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>194</v>
+      </c>
+      <c r="J6" s="41" t="s">
+        <v>195</v>
+      </c>
+      <c r="K6" s="41" t="s">
+        <v>196</v>
+      </c>
+      <c r="L6" s="28" t="s">
+        <v>197</v>
+      </c>
+      <c r="M6" s="28" t="s">
+        <v>195</v>
+      </c>
+      <c r="O6" s="28" t="s">
+        <v>198</v>
+      </c>
+      <c r="P6" s="28" t="s">
+        <v>199</v>
+      </c>
+      <c r="Q6" s="28" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" s="36" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="36">
+        <v>301</v>
+      </c>
+      <c r="B7" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C7" s="37" t="s">
+        <v>437</v>
+      </c>
+      <c r="D7" s="38">
+        <v>1</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37" t="s">
+        <v>438</v>
+      </c>
+      <c r="H7" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="I7" s="36">
+        <v>1</v>
+      </c>
+      <c r="J7" s="36">
+        <f>IF(I7&gt;D7,0,D7-I7)</f>
+        <v>0</v>
+      </c>
+      <c r="K7" s="36">
+        <f>I7+J7</f>
+        <v>1</v>
+      </c>
+      <c r="L7" s="36">
+        <f>K7-D7</f>
+        <v>0</v>
+      </c>
+      <c r="M7" s="36">
+        <f>(4*D7)-L7</f>
+        <v>4</v>
+      </c>
+      <c r="O7" s="28"/>
+      <c r="P7" s="28"/>
+      <c r="Q7" s="28"/>
+    </row>
+    <row r="8" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A8" s="41">
+        <v>302</v>
+      </c>
+      <c r="B8" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C8" s="46" t="s">
+        <v>440</v>
+      </c>
+      <c r="D8" s="38">
+        <v>1</v>
+      </c>
+      <c r="E8" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q8" s="43"/>
+    </row>
+    <row r="9" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A9" s="36">
+        <v>303</v>
+      </c>
+      <c r="B9" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>441</v>
+      </c>
+      <c r="D9" s="38">
+        <v>1</v>
+      </c>
+      <c r="E9" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H9" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q9" s="43"/>
+    </row>
+    <row r="10" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="41">
+        <v>304</v>
+      </c>
+      <c r="B10" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C10" s="46" t="s">
+        <v>442</v>
+      </c>
+      <c r="D10" s="38">
+        <v>1</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H10" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q10" s="43"/>
+    </row>
+    <row r="11" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A11" s="36">
+        <v>305</v>
+      </c>
+      <c r="B11" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C11" s="46" t="s">
+        <v>443</v>
+      </c>
+      <c r="D11" s="38">
+        <v>1</v>
+      </c>
+      <c r="E11" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H11" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="I11" s="44"/>
+      <c r="J11" s="44"/>
+      <c r="P11" s="45"/>
+      <c r="Q11" s="43"/>
+    </row>
+    <row r="12" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="41">
+        <v>306</v>
+      </c>
+      <c r="B12" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C12" s="46" t="s">
+        <v>445</v>
+      </c>
+      <c r="D12" s="38">
+        <v>1</v>
+      </c>
+      <c r="E12" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H12" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="I12" s="44"/>
+      <c r="J12" s="44"/>
+      <c r="P12" s="45"/>
+      <c r="Q12" s="43"/>
+    </row>
+    <row r="13" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="36">
+        <v>307</v>
+      </c>
+      <c r="B13" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C13" s="46" t="s">
+        <v>446</v>
+      </c>
+      <c r="D13" s="38">
+        <v>1</v>
+      </c>
+      <c r="E13" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q13" s="43"/>
+    </row>
+    <row r="14" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="41">
+        <v>308</v>
+      </c>
+      <c r="B14" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C14" s="46" t="s">
+        <v>444</v>
+      </c>
+      <c r="D14" s="38">
+        <v>1</v>
+      </c>
+      <c r="E14" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="G14" s="46" t="s">
+        <v>449</v>
+      </c>
+      <c r="H14" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="I14" s="41">
+        <v>4</v>
+      </c>
+      <c r="J14" s="41">
+        <v>0</v>
+      </c>
+      <c r="K14" s="36">
+        <f>I14+J14</f>
+        <v>4</v>
+      </c>
+      <c r="L14" s="36">
+        <f>K14-D14</f>
+        <v>3</v>
+      </c>
+      <c r="M14" s="36">
+        <f>(4*D14)-L14</f>
+        <v>1</v>
+      </c>
+      <c r="Q14" s="43"/>
+    </row>
+    <row r="15" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A15" s="36">
+        <v>309</v>
+      </c>
+      <c r="B15" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C15" s="46" t="s">
+        <v>447</v>
+      </c>
+      <c r="D15" s="38">
+        <v>1</v>
+      </c>
+      <c r="E15" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H15" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q15" s="43"/>
+    </row>
+    <row r="16" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A16" s="41">
+        <v>310</v>
+      </c>
+      <c r="B16" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C16" s="46" t="s">
+        <v>448</v>
+      </c>
+      <c r="D16" s="38">
+        <v>1</v>
+      </c>
+      <c r="E16" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H16" s="36" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q16" s="43"/>
+    </row>
+    <row r="17" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q17" s="43"/>
+    </row>
+    <row r="18" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q18" s="43"/>
+    </row>
+    <row r="19" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q19" s="43"/>
+    </row>
+    <row r="20" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q20" s="43"/>
+    </row>
+    <row r="21" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q21" s="43"/>
+    </row>
+    <row r="22" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q22" s="43"/>
+    </row>
+    <row r="23" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q23" s="43"/>
+    </row>
+    <row r="24" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q24" s="43"/>
+    </row>
+    <row r="25" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+  </sheetData>
+  <autoFilter ref="A6:M31" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:M31">
+      <sortCondition ref="B6:B31"/>
+    </sortState>
+  </autoFilter>
+  <mergeCells count="1">
+    <mergeCell ref="O3:Q3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
BOM refinement after Core Board prototype is soldered.
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25A8226B-066C-E048-B34F-EE5078BB5DC6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF4AC2C-35E7-FC43-9CE9-878460F360C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33840" windowHeight="21580" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2440" windowWidth="37640" windowHeight="20000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept Estimate" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Core Board V0.3'!$A$6:$M$31</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Middle Layers'!$A$6:$M$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Middle Layers'!$A$6:$M$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="805" uniqueCount="450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="823" uniqueCount="460">
   <si>
     <t>Digi-Key Part Number</t>
   </si>
@@ -1393,6 +1393,36 @@
   </si>
   <si>
     <t>Pimoroni Unicorn Hat</t>
+  </si>
+  <si>
+    <t>Glue magnet to stylus</t>
+  </si>
+  <si>
+    <t>Lanyard</t>
+  </si>
+  <si>
+    <t>Not labeled - for Adafruit MicroSD Breakout</t>
+  </si>
+  <si>
+    <t>user cuts to size 85x85mm</t>
+  </si>
+  <si>
+    <t>user glues it</t>
+  </si>
+  <si>
+    <t>AAA batteries</t>
+  </si>
+  <si>
+    <t>user installs</t>
+  </si>
+  <si>
+    <t>Solder paste</t>
+  </si>
+  <si>
+    <t>Solder paste, Syringe</t>
+  </si>
+  <si>
+    <t>Solder paste, Syringe Tip</t>
   </si>
 </sst>
 </file>
@@ -1404,10 +1434,24 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1434,6 +1478,20 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -1538,36 +1596,36 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="44" fontId="5" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1577,66 +1635,99 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4392,14 +4483,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5DBFB5-E21A-7B4B-815F-748A526FD280}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="125" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8:P12"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12:M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="28"/>
-    <col min="2" max="2" width="17" style="28" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" style="28" customWidth="1"/>
     <col min="3" max="3" width="39.6640625" style="28" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" style="28" customWidth="1"/>
@@ -4434,11 +4525,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="O3" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -4495,13 +4586,13 @@
       <c r="A6" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="B6" s="28" t="s">
+      <c r="B6" s="30" t="s">
         <v>189</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="30" t="s">
         <v>190</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="30" t="s">
         <v>148</v>
       </c>
       <c r="E6" s="28" t="s">
@@ -4545,13 +4636,13 @@
       <c r="A7" s="28">
         <v>4</v>
       </c>
-      <c r="B7" s="28" t="s">
+      <c r="B7" s="30" t="s">
         <v>201</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="30">
         <v>8</v>
       </c>
       <c r="E7" s="28" t="s">
@@ -4560,7 +4651,7 @@
       <c r="F7" s="28" t="s">
         <v>204</v>
       </c>
-      <c r="G7" s="28" t="s">
+      <c r="G7" s="30" t="s">
         <v>205</v>
       </c>
       <c r="H7" s="28" t="s">
@@ -4573,7 +4664,7 @@
         <f>IF(I7&gt;D7,0,D7-I7)</f>
         <v>6</v>
       </c>
-      <c r="K7" s="28">
+      <c r="K7" s="30">
         <f>I7+J7</f>
         <v>8</v>
       </c>
@@ -4594,13 +4685,13 @@
       <c r="A8" s="28">
         <v>5</v>
       </c>
-      <c r="B8" s="28" t="s">
+      <c r="B8" s="30" t="s">
         <v>207</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="30" t="s">
         <v>202</v>
       </c>
-      <c r="D8" s="28">
+      <c r="D8" s="30">
         <v>4</v>
       </c>
       <c r="E8" s="28" t="s">
@@ -4609,29 +4700,29 @@
       <c r="F8" s="28" t="s">
         <v>208</v>
       </c>
-      <c r="G8" s="28" t="s">
+      <c r="G8" s="30" t="s">
         <v>209</v>
       </c>
       <c r="H8" s="28" t="s">
         <v>206</v>
       </c>
       <c r="I8" s="28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" s="30">
         <v>10</v>
       </c>
-      <c r="K8" s="28">
+      <c r="K8" s="30">
         <f t="shared" ref="K8:K24" si="3">I8+J8</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L8" s="28">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="M8" s="28">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Q8" s="32" t="e">
         <f t="shared" si="2"/>
@@ -4827,15 +4918,15 @@
         <f>2450/3.281</f>
         <v>746.72355989027733</v>
       </c>
-      <c r="K12" s="28">
+      <c r="K12" s="33">
         <f t="shared" si="3"/>
         <v>746.72355989027733</v>
       </c>
-      <c r="L12" s="28">
+      <c r="L12" s="33">
         <f t="shared" si="0"/>
         <v>745.97355989027733</v>
       </c>
-      <c r="M12" s="28">
+      <c r="M12" s="33">
         <f t="shared" si="1"/>
         <v>-742.97355989027733</v>
       </c>
@@ -4907,7 +4998,7 @@
       <c r="C14" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="D14" s="28">
+      <c r="D14" s="30">
         <v>1</v>
       </c>
       <c r="E14" s="28" t="s">
@@ -4947,10 +5038,10 @@
       <c r="A15" s="28">
         <v>101</v>
       </c>
-      <c r="B15" s="28" t="s">
+      <c r="B15" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="30" t="s">
         <v>230</v>
       </c>
       <c r="D15" s="30">
@@ -4996,13 +5087,13 @@
       <c r="A16" s="28">
         <v>6</v>
       </c>
-      <c r="B16" s="28" t="s">
+      <c r="B16" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="30" t="s">
         <v>233</v>
       </c>
-      <c r="D16" s="28">
+      <c r="D16" s="30">
         <v>4</v>
       </c>
       <c r="E16" s="28" t="s">
@@ -5042,10 +5133,10 @@
       <c r="A17" s="28">
         <v>11</v>
       </c>
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="30" t="s">
         <v>236</v>
       </c>
       <c r="D17" s="30">
@@ -5088,10 +5179,10 @@
       <c r="A18" s="28">
         <v>12</v>
       </c>
-      <c r="B18" s="28" t="s">
+      <c r="B18" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="30" t="s">
         <v>236</v>
       </c>
       <c r="D18" s="30">
@@ -5134,10 +5225,10 @@
       <c r="A19" s="28">
         <v>14</v>
       </c>
-      <c r="B19" s="28" t="s">
+      <c r="B19" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="30" t="s">
         <v>236</v>
       </c>
       <c r="D19" s="30">
@@ -5180,10 +5271,10 @@
       <c r="A20" s="28">
         <v>7</v>
       </c>
-      <c r="B20" s="28" t="s">
+      <c r="B20" s="30" t="s">
         <v>242</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="30" t="s">
         <v>243</v>
       </c>
       <c r="D20" s="30">
@@ -5226,10 +5317,10 @@
       <c r="A21" s="28">
         <v>8</v>
       </c>
-      <c r="B21" s="28" t="s">
+      <c r="B21" s="30" t="s">
         <v>245</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="30" t="s">
         <v>243</v>
       </c>
       <c r="D21" s="30">
@@ -5272,10 +5363,10 @@
       <c r="A22" s="28">
         <v>9</v>
       </c>
-      <c r="B22" s="28" t="s">
+      <c r="B22" s="30" t="s">
         <v>247</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="30" t="s">
         <v>243</v>
       </c>
       <c r="D22" s="30">
@@ -5318,10 +5409,10 @@
       <c r="A23" s="28">
         <v>10</v>
       </c>
-      <c r="B23" s="28" t="s">
+      <c r="B23" s="30" t="s">
         <v>249</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="30" t="s">
         <v>243</v>
       </c>
       <c r="D23" s="30">
@@ -5458,8 +5549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59:XFD59"/>
+    <sheetView topLeftCell="A27" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5527,11 +5618,11 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="O7" s="42" t="s">
+      <c r="O7" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="42"/>
+      <c r="P7" s="56"/>
+      <c r="Q7" s="56"/>
     </row>
     <row r="8" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -5714,20 +5805,20 @@
         <v>2</v>
       </c>
       <c r="K11" s="28">
-        <f>I11+J11</f>
+        <f t="shared" ref="K11:K17" si="0">I11+J11</f>
         <v>2</v>
       </c>
       <c r="L11" s="28">
-        <f>K11-D11</f>
+        <f t="shared" ref="L11:L17" si="1">K11-D11</f>
         <v>0</v>
       </c>
       <c r="M11" s="28">
-        <f>(4*D11)-L11</f>
+        <f t="shared" ref="M11:M17" si="2">(4*D11)-L11</f>
         <v>8</v>
       </c>
       <c r="N11" s="28"/>
       <c r="Q11" s="32" t="e">
-        <f>P11/O11</f>
+        <f t="shared" ref="Q11:Q28" si="3">P11/O11</f>
         <v>#DIV/0!</v>
       </c>
       <c r="R11" s="36" t="s">
@@ -5769,21 +5860,21 @@
         <f>IF(I12&gt;D12,0,D12-I12)</f>
         <v>7</v>
       </c>
-      <c r="K12" s="28">
-        <f>I12+J12</f>
+      <c r="K12" s="30">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="L12" s="28">
-        <f>K12-D12</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M12" s="28">
-        <f>(4*D12)-L12</f>
+        <f t="shared" si="2"/>
         <v>28</v>
       </c>
       <c r="N12" s="28"/>
       <c r="Q12" s="32" t="e">
-        <f>P12/O12</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R12" s="36" t="s">
@@ -5825,20 +5916,20 @@
         <v>10</v>
       </c>
       <c r="K13" s="28">
-        <f>I13+J13</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="L13" s="28">
-        <f>K13-D13</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="M13" s="28">
-        <f>(4*D13)-L13</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="N13" s="28"/>
       <c r="Q13" s="32" t="e">
-        <f>P13/O13</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R13" s="36" t="s">
@@ -5881,15 +5972,15 @@
         <v>0</v>
       </c>
       <c r="K14" s="28">
-        <f>I14+J14</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L14" s="28">
-        <f>K14-D14</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M14" s="28">
-        <f>(4*D14)-L14</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="N14" s="28"/>
@@ -5897,7 +5988,7 @@
         <v>430</v>
       </c>
       <c r="Q14" s="32">
-        <f>P14/O14</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R14" s="36" t="s">
@@ -5940,15 +6031,15 @@
         <v>2</v>
       </c>
       <c r="K15" s="28">
-        <f>I15+J15</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L15" s="28">
-        <f>K15-D15</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M15" s="28">
-        <f>(4*D15)-L15</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="N15" s="28"/>
@@ -5957,7 +6048,7 @@
       </c>
       <c r="P15" s="35"/>
       <c r="Q15" s="32">
-        <f>P15/O15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R15" s="36" t="s">
@@ -6000,15 +6091,15 @@
         <v>2</v>
       </c>
       <c r="K16" s="28">
-        <f>I16+J16</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="L16" s="28">
-        <f>K16-D16</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M16" s="28">
-        <f>(4*D16)-L16</f>
+        <f t="shared" si="2"/>
         <v>24</v>
       </c>
       <c r="N16" s="28"/>
@@ -6017,7 +6108,7 @@
       </c>
       <c r="P16" s="35"/>
       <c r="Q16" s="32">
-        <f>P16/O16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="R16" s="36" t="s">
@@ -6060,20 +6151,20 @@
         <v>0</v>
       </c>
       <c r="K17" s="28">
-        <f>I17+J17</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="L17" s="28">
-        <f>K17-D17</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M17" s="28">
-        <f>(4*D17)-L17</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="N17" s="28"/>
       <c r="Q17" s="32" t="e">
-        <f>P17/O17</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R17" s="36" t="s">
@@ -6098,7 +6189,7 @@
       <c r="M18" s="28"/>
       <c r="N18" s="28"/>
       <c r="Q18" s="32" t="e">
-        <f>P18/O18</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S18" s="36" t="s">
@@ -6120,7 +6211,7 @@
       <c r="M19" s="28"/>
       <c r="N19" s="28"/>
       <c r="Q19" s="32" t="e">
-        <f>P19/O19</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="S19" s="36" t="s">
@@ -6173,7 +6264,7 @@
       </c>
       <c r="N20" s="28"/>
       <c r="Q20" s="32" t="e">
-        <f>P20/O20</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R20" s="36" t="s">
@@ -6241,7 +6332,7 @@
       </c>
       <c r="N21" s="28"/>
       <c r="Q21" s="32" t="e">
-        <f>P21/O21</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R21" s="36" t="s">
@@ -6297,7 +6388,7 @@
       </c>
       <c r="N22" s="28"/>
       <c r="Q22" s="32" t="e">
-        <f>P22/O22</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R22" s="36" t="s">
@@ -6353,7 +6444,7 @@
       </c>
       <c r="N23" s="28"/>
       <c r="Q23" s="32" t="e">
-        <f>P23/O23</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R23" s="36" t="s">
@@ -6409,7 +6500,7 @@
       </c>
       <c r="N24" s="28"/>
       <c r="Q24" s="32" t="e">
-        <f>P24/O24</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
       <c r="R24" s="36" t="s">
@@ -6434,7 +6525,7 @@
       <c r="M25" s="28"/>
       <c r="N25" s="28"/>
       <c r="Q25" s="32" t="e">
-        <f>P25/O25</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6453,7 +6544,7 @@
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
       <c r="Q26" s="32" t="e">
-        <f>P26/O26</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6472,7 +6563,7 @@
       <c r="M27" s="28"/>
       <c r="N27" s="28"/>
       <c r="Q27" s="32" t="e">
-        <f>P27/O27</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6491,7 +6582,7 @@
       <c r="M28" s="28"/>
       <c r="N28" s="28"/>
       <c r="Q28" s="32" t="e">
-        <f>P28/O28</f>
+        <f t="shared" si="3"/>
         <v>#DIV/0!</v>
       </c>
     </row>
@@ -6558,15 +6649,15 @@
         <v>0</v>
       </c>
       <c r="K31" s="28">
-        <f>I31+J31</f>
+        <f t="shared" ref="K31:K58" si="4">I31+J31</f>
         <v>1</v>
       </c>
       <c r="L31" s="28">
-        <f>K31-D31</f>
+        <f t="shared" ref="L31:L58" si="5">K31-D31</f>
         <v>0</v>
       </c>
       <c r="M31" s="28">
-        <f>(4*D31)-L31</f>
+        <f t="shared" ref="M31:M58" si="6">(4*D31)-L31</f>
         <v>4</v>
       </c>
       <c r="N31" s="28"/>
@@ -6609,15 +6700,15 @@
         <v>10</v>
       </c>
       <c r="K32" s="28">
-        <f>I32+J32</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="L32" s="28">
-        <f>K32-D32</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="M32" s="28">
-        <f>(4*D32)-L32</f>
+        <f t="shared" si="6"/>
         <v>38</v>
       </c>
       <c r="N32" s="28"/>
@@ -6684,15 +6775,15 @@
         <v>10</v>
       </c>
       <c r="K33" s="28">
-        <f>I33+J33</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="L33" s="28">
-        <f>K33-D33</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M33" s="28">
-        <f>(4*D33)-L33</f>
+        <f t="shared" si="6"/>
         <v>43</v>
       </c>
       <c r="N33" s="28"/>
@@ -6758,15 +6849,15 @@
         <v>0</v>
       </c>
       <c r="K34" s="28">
-        <f>I34+J34</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L34" s="28">
-        <f>K34-D34</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M34" s="28">
-        <f>(4*D34)-L34</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N34" s="28"/>
@@ -6809,15 +6900,15 @@
         <v>10</v>
       </c>
       <c r="K35" s="28">
-        <f>I35+J35</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="L35" s="28">
-        <f>K35-D35</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="M35" s="28">
-        <f>(4*D35)-L35</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N35" s="28"/>
@@ -6858,15 +6949,15 @@
       </c>
       <c r="J36" s="40"/>
       <c r="K36" s="28">
-        <f>I36+J36</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="L36" s="28">
-        <f>K36-D36</f>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="M36" s="28">
-        <f>(4*D36)-L36</f>
+        <f t="shared" si="6"/>
         <v>5</v>
       </c>
       <c r="N36" s="28"/>
@@ -6909,15 +7000,15 @@
         <v>20</v>
       </c>
       <c r="K37" s="28">
-        <f>I37+J37</f>
+        <f t="shared" si="4"/>
         <v>31</v>
       </c>
       <c r="L37" s="28">
-        <f>K37-D37</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
       <c r="M37" s="28">
-        <f>(4*D37)-L37</f>
+        <f t="shared" si="6"/>
         <v>74</v>
       </c>
       <c r="N37" s="28"/>
@@ -6960,15 +7051,15 @@
         <v>10</v>
       </c>
       <c r="K38" s="28">
-        <f>I38+J38</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="L38" s="28">
-        <f>K38-D38</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="M38" s="28">
-        <f>(4*D38)-L38</f>
+        <f t="shared" si="6"/>
         <v>16</v>
       </c>
       <c r="N38" s="28"/>
@@ -7012,15 +7103,15 @@
         <v>0</v>
       </c>
       <c r="K39" s="28">
-        <f>I39+J39</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L39" s="28">
-        <f>K39-D39</f>
+        <f t="shared" si="5"/>
         <v>5</v>
       </c>
       <c r="M39" s="28">
-        <f>(4*D39)-L39</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="N39" s="28"/>
@@ -7064,15 +7155,15 @@
         <v>0</v>
       </c>
       <c r="K40" s="28">
-        <f>I40+J40</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="L40" s="28">
-        <f>K40-D40</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
       <c r="M40" s="28">
-        <f>(4*D40)-L40</f>
+        <f t="shared" si="6"/>
         <v>2</v>
       </c>
       <c r="N40" s="28"/>
@@ -7115,15 +7206,15 @@
         <v>10</v>
       </c>
       <c r="K41" s="28">
-        <f>I41+J41</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="L41" s="28">
-        <f>K41-D41</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
       <c r="M41" s="28">
-        <f>(4*D41)-L41</f>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="N41" s="28"/>
@@ -7163,19 +7254,19 @@
         <v>6</v>
       </c>
       <c r="J42" s="28">
-        <f>IF(I42&gt;D42,0,D42-I42)</f>
+        <f t="shared" ref="J42:J58" si="7">IF(I42&gt;D42,0,D42-I42)</f>
         <v>0</v>
       </c>
       <c r="K42" s="28">
-        <f>I42+J42</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="L42" s="28">
-        <f>K42-D42</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M42" s="28">
-        <f>(4*D42)-L42</f>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
       <c r="N42" s="28"/>
@@ -7215,19 +7306,19 @@
         <v>1</v>
       </c>
       <c r="J43" s="28">
-        <f>IF(I43&gt;D43,0,D43-I43)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K43" s="28">
-        <f>I43+J43</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L43" s="28">
-        <f>K43-D43</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M43" s="28">
-        <f>(4*D43)-L43</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N43" s="28"/>
@@ -7267,19 +7358,19 @@
         <v>1</v>
       </c>
       <c r="J44" s="28">
-        <f>IF(I44&gt;D44,0,D44-I44)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K44" s="28">
-        <f>I44+J44</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L44" s="28">
-        <f>K44-D44</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M44" s="28">
-        <f>(4*D44)-L44</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N44" s="28"/>
@@ -7317,19 +7408,19 @@
         <v>2</v>
       </c>
       <c r="J45" s="28">
-        <f>IF(I45&gt;D45,0,D45-I45)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K45" s="28">
-        <f>I45+J45</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L45" s="28">
-        <f>K45-D45</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
       <c r="M45" s="28">
-        <f>(4*D45)-L45</f>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
       <c r="N45" s="28"/>
@@ -7366,19 +7457,19 @@
         <v>0</v>
       </c>
       <c r="J46" s="30">
-        <f>IF(I46&gt;D46,0,D46-I46)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="K46" s="28">
-        <f>I46+J46</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L46" s="28">
-        <f>K46-D46</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M46" s="28">
-        <f>(4*D46)-L46</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N46" s="28"/>
@@ -7418,19 +7509,19 @@
         <v>1</v>
       </c>
       <c r="J47" s="28">
-        <f>IF(I47&gt;D47,0,D47-I47)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K47" s="28">
-        <f>I47+J47</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L47" s="28">
-        <f>K47-D47</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M47" s="28">
-        <f>(4*D47)-L47</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N47" s="28"/>
@@ -7470,19 +7561,19 @@
         <v>2</v>
       </c>
       <c r="J48" s="28">
-        <f>IF(I48&gt;D48,0,D48-I48)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K48" s="28">
-        <f>I48+J48</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L48" s="28">
-        <f>K48-D48</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M48" s="28">
-        <f>(4*D48)-L48</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="N48" s="28"/>
@@ -7522,19 +7613,19 @@
         <v>1</v>
       </c>
       <c r="J49" s="28">
-        <f>IF(I49&gt;D49,0,D49-I49)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K49" s="28">
-        <f>I49+J49</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L49" s="28">
-        <f>K49-D49</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M49" s="28">
-        <f>(4*D49)-L49</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N49" s="28"/>
@@ -7574,19 +7665,19 @@
         <v>1</v>
       </c>
       <c r="J50" s="28">
-        <f>IF(I50&gt;D50,0,D50-I50)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K50" s="28">
-        <f>I50+J50</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L50" s="28">
-        <f>K50-D50</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M50" s="28">
-        <f>(4*D50)-L50</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N50" s="28"/>
@@ -7626,19 +7717,19 @@
         <v>1</v>
       </c>
       <c r="J51" s="28">
-        <f>IF(I51&gt;D51,0,D51-I51)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K51" s="28">
-        <f>I51+J51</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L51" s="28">
-        <f>K51-D51</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M51" s="28">
-        <f>(4*D51)-L51</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N51" s="28"/>
@@ -7678,19 +7769,19 @@
         <v>1</v>
       </c>
       <c r="J52" s="28">
-        <f>IF(I52&gt;D52,0,D52-I52)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K52" s="28">
-        <f>I52+J52</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L52" s="28">
-        <f>K52-D52</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M52" s="28">
-        <f>(4*D52)-L52</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N52" s="28"/>
@@ -7728,19 +7819,19 @@
         <v>1</v>
       </c>
       <c r="J53" s="28">
-        <f>IF(I53&gt;D53,0,D53-I53)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K53" s="28">
-        <f>I53+J53</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L53" s="28">
-        <f>K53-D53</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M53" s="28">
-        <f>(4*D53)-L53</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N53" s="28"/>
@@ -7752,6 +7843,9 @@
       <c r="A54" s="36">
         <v>101</v>
       </c>
+      <c r="B54" s="55" t="s">
+        <v>452</v>
+      </c>
       <c r="D54" s="38">
         <v>1</v>
       </c>
@@ -7768,19 +7862,19 @@
         <v>0</v>
       </c>
       <c r="J54" s="30">
-        <f>IF(I54&gt;D54,0,D54-I54)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="K54" s="28">
-        <f>I54+J54</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L54" s="28">
-        <f>K54-D54</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M54" s="28">
-        <f>(4*D54)-L54</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
       <c r="N54" s="28"/>
@@ -7814,19 +7908,19 @@
         <v>0</v>
       </c>
       <c r="J55" s="30">
-        <f>IF(I55&gt;D55,0,D55-I55)</f>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="K55" s="28">
-        <f>I55+J55</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L55" s="28">
-        <f>K55-D55</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M55" s="28">
-        <f>(4*D55)-L55</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="N55" s="28"/>
@@ -7860,19 +7954,19 @@
         <v>2</v>
       </c>
       <c r="J56" s="28">
-        <f>IF(I56&gt;D56,0,D56-I56)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K56" s="28">
-        <f>I56+J56</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="L56" s="28">
-        <f>K56-D56</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M56" s="28">
-        <f>(4*D56)-L56</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="N56" s="28"/>
@@ -7912,19 +8006,19 @@
         <v>1</v>
       </c>
       <c r="J57" s="36">
-        <f>IF(I57&gt;D57,0,D57-I57)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K57" s="36">
-        <f>I57+J57</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="L57" s="36">
-        <f>K57-D57</f>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="M57" s="36">
-        <f>(4*D57)-L57</f>
+        <f t="shared" si="6"/>
         <v>4</v>
       </c>
     </row>
@@ -7951,23 +8045,46 @@
         <v>5</v>
       </c>
       <c r="J58" s="36">
-        <f>IF(I58&gt;D58,0,D58-I58)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="K58" s="36">
-        <f>I58+J58</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="L58" s="36">
-        <f>K58-D58</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
       <c r="M58" s="36">
-        <f>(4*D58)-L58</f>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" ht="17" x14ac:dyDescent="0.2">
+      <c r="A59" s="36">
+        <v>106</v>
+      </c>
+      <c r="B59" s="36" t="s">
+        <v>431</v>
+      </c>
+      <c r="C59" s="54" t="s">
+        <v>451</v>
+      </c>
+      <c r="D59" s="38">
+        <v>1</v>
+      </c>
+      <c r="E59" s="28" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A60" s="36">
+        <v>107</v>
+      </c>
+      <c r="B60" s="57" t="s">
+        <v>457</v>
+      </c>
       <c r="J60" s="36">
         <f>IF(I60&gt;D60,0,D60-I60)</f>
         <v>0</v>
@@ -7986,6 +8103,12 @@
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A61" s="36">
+        <v>108</v>
+      </c>
+      <c r="B61" s="57" t="s">
+        <v>458</v>
+      </c>
       <c r="J61" s="36">
         <f>IF(I61&gt;D61,0,D61-I61)</f>
         <v>0</v>
@@ -8004,6 +8127,12 @@
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A62" s="36">
+        <v>109</v>
+      </c>
+      <c r="B62" s="57" t="s">
+        <v>459</v>
+      </c>
       <c r="J62" s="36">
         <f>IF(I62&gt;D62,0,D62-I62)</f>
         <v>0</v>
@@ -8031,10 +8160,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87AFCDAF-E620-294C-BC98-AFD17B703801}">
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:Q30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -8044,7 +8173,7 @@
     <col min="3" max="3" width="39.6640625" style="28" customWidth="1"/>
     <col min="4" max="4" width="12.1640625" style="28" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.83203125" style="28" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" style="28" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" style="28" customWidth="1"/>
     <col min="7" max="7" width="28.5" style="28" customWidth="1"/>
     <col min="8" max="8" width="9.6640625" style="28" customWidth="1"/>
     <col min="9" max="9" width="28" style="28" customWidth="1"/>
@@ -8075,11 +8204,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="O3" s="56" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="42"/>
-      <c r="Q3" s="42"/>
+      <c r="P3" s="56"/>
+      <c r="Q3" s="56"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -8235,7 +8364,7 @@
       <c r="B8" s="36" t="s">
         <v>436</v>
       </c>
-      <c r="C8" s="46" t="s">
+      <c r="C8" s="45" t="s">
         <v>440</v>
       </c>
       <c r="D8" s="38">
@@ -8247,7 +8376,7 @@
       <c r="H8" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="Q8" s="43"/>
+      <c r="Q8" s="42"/>
     </row>
     <row r="9" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="36">
@@ -8256,7 +8385,7 @@
       <c r="B9" s="36" t="s">
         <v>436</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="45" t="s">
         <v>441</v>
       </c>
       <c r="D9" s="38">
@@ -8268,28 +8397,28 @@
       <c r="H9" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="Q9" s="43"/>
-    </row>
-    <row r="10" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A10" s="41">
+      <c r="Q9" s="42"/>
+    </row>
+    <row r="10" spans="1:17" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A10" s="47">
         <v>304</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="47" t="s">
         <v>442</v>
       </c>
-      <c r="D10" s="38">
-        <v>1</v>
-      </c>
-      <c r="E10" s="28" t="s">
+      <c r="D10" s="49">
+        <v>1</v>
+      </c>
+      <c r="E10" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="H10" s="36" t="s">
+      <c r="H10" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="Q10" s="43"/>
+      <c r="Q10" s="53"/>
     </row>
     <row r="11" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="36">
@@ -8298,7 +8427,7 @@
       <c r="B11" s="36" t="s">
         <v>436</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="45" t="s">
         <v>443</v>
       </c>
       <c r="D11" s="38">
@@ -8310,55 +8439,55 @@
       <c r="H11" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="I11" s="44"/>
-      <c r="J11" s="44"/>
-      <c r="P11" s="45"/>
-      <c r="Q11" s="43"/>
-    </row>
-    <row r="12" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="41">
+      <c r="I11" s="43"/>
+      <c r="J11" s="43"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="42"/>
+    </row>
+    <row r="12" spans="1:17" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A12" s="47">
         <v>306</v>
       </c>
-      <c r="B12" s="36" t="s">
+      <c r="B12" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="47" t="s">
         <v>445</v>
       </c>
-      <c r="D12" s="38">
-        <v>1</v>
-      </c>
-      <c r="E12" s="28" t="s">
+      <c r="D12" s="49">
+        <v>1</v>
+      </c>
+      <c r="E12" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="I12" s="44"/>
-      <c r="J12" s="44"/>
-      <c r="P12" s="45"/>
-      <c r="Q12" s="43"/>
-    </row>
-    <row r="13" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A13" s="36">
+      <c r="I12" s="51"/>
+      <c r="J12" s="51"/>
+      <c r="P12" s="52"/>
+      <c r="Q12" s="53"/>
+    </row>
+    <row r="13" spans="1:17" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A13" s="48">
         <v>307</v>
       </c>
-      <c r="B13" s="36" t="s">
+      <c r="B13" s="48" t="s">
         <v>436</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="47" t="s">
         <v>446</v>
       </c>
-      <c r="D13" s="38">
-        <v>1</v>
-      </c>
-      <c r="E13" s="28" t="s">
+      <c r="D13" s="49">
+        <v>1</v>
+      </c>
+      <c r="E13" s="50" t="s">
         <v>203</v>
       </c>
-      <c r="H13" s="36" t="s">
+      <c r="H13" s="48" t="s">
         <v>206</v>
       </c>
-      <c r="Q13" s="43"/>
+      <c r="Q13" s="53"/>
     </row>
     <row r="14" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="41">
@@ -8367,7 +8496,7 @@
       <c r="B14" s="36" t="s">
         <v>436</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="45" t="s">
         <v>444</v>
       </c>
       <c r="D14" s="38">
@@ -8376,7 +8505,7 @@
       <c r="E14" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="G14" s="46" t="s">
+      <c r="G14" s="45" t="s">
         <v>449</v>
       </c>
       <c r="H14" s="36" t="s">
@@ -8400,7 +8529,7 @@
         <f>(4*D14)-L14</f>
         <v>1</v>
       </c>
-      <c r="Q14" s="43"/>
+      <c r="Q14" s="42"/>
     </row>
     <row r="15" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="36">
@@ -8409,7 +8538,7 @@
       <c r="B15" s="36" t="s">
         <v>436</v>
       </c>
-      <c r="C15" s="46" t="s">
+      <c r="C15" s="45" t="s">
         <v>447</v>
       </c>
       <c r="D15" s="38">
@@ -8418,10 +8547,13 @@
       <c r="E15" s="28" t="s">
         <v>203</v>
       </c>
+      <c r="F15" s="46" t="s">
+        <v>453</v>
+      </c>
       <c r="H15" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="Q15" s="43"/>
+      <c r="Q15" s="42"/>
     </row>
     <row r="16" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="41">
@@ -8430,7 +8562,7 @@
       <c r="B16" s="36" t="s">
         <v>436</v>
       </c>
-      <c r="C16" s="46" t="s">
+      <c r="C16" s="45" t="s">
         <v>448</v>
       </c>
       <c r="D16" s="38">
@@ -8439,46 +8571,82 @@
       <c r="E16" s="28" t="s">
         <v>203</v>
       </c>
+      <c r="F16" s="46" t="s">
+        <v>453</v>
+      </c>
       <c r="H16" s="36" t="s">
         <v>206</v>
       </c>
-      <c r="Q16" s="43"/>
-    </row>
-    <row r="17" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="Q17" s="43"/>
-    </row>
-    <row r="18" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="Q18" s="43"/>
-    </row>
-    <row r="19" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="Q19" s="43"/>
-    </row>
-    <row r="20" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="Q20" s="43"/>
-    </row>
-    <row r="21" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="Q21" s="43"/>
-    </row>
-    <row r="22" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="Q22" s="43"/>
-    </row>
-    <row r="23" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="Q23" s="43"/>
-    </row>
-    <row r="24" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
-      <c r="Q24" s="43"/>
-    </row>
-    <row r="25" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="26" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="27" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="28" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="30" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
-    <row r="31" spans="17:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+      <c r="Q16" s="42"/>
+    </row>
+    <row r="17" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="41">
+        <v>311</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C17" s="46" t="s">
+        <v>450</v>
+      </c>
+      <c r="F17" s="46" t="s">
+        <v>454</v>
+      </c>
+      <c r="H17" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q17" s="42"/>
+    </row>
+    <row r="18" spans="1:17" s="41" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="41">
+        <v>312</v>
+      </c>
+      <c r="B18" s="36" t="s">
+        <v>436</v>
+      </c>
+      <c r="C18" s="46" t="s">
+        <v>455</v>
+      </c>
+      <c r="D18" s="38">
+        <v>1</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>203</v>
+      </c>
+      <c r="F18" s="46" t="s">
+        <v>456</v>
+      </c>
+      <c r="H18" s="46" t="s">
+        <v>206</v>
+      </c>
+      <c r="Q18" s="42"/>
+    </row>
+    <row r="19" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q19" s="42"/>
+    </row>
+    <row r="20" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q20" s="42"/>
+    </row>
+    <row r="21" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q21" s="42"/>
+    </row>
+    <row r="22" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q22" s="42"/>
+    </row>
+    <row r="23" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="Q23" s="42"/>
+    </row>
+    <row r="24" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="25" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="26" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="27" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="28" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="29" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
+    <row r="30" spans="1:17" s="41" customFormat="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <autoFilter ref="A6:M31" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:M31">
-      <sortCondition ref="B6:B31"/>
+  <autoFilter ref="A6:M30" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A7:M30">
+      <sortCondition ref="B6:B30"/>
     </sortState>
   </autoFilter>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add my chip addresses to I2C scanner.
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BF4AC2C-35E7-FC43-9CE9-878460F360C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A806B6-63DC-764E-A98F-9E45F6DDFCDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="2440" windowWidth="37640" windowHeight="20000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1434,10 +1434,17 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1596,36 +1603,36 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1635,99 +1642,102 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4484,7 +4494,7 @@
   <dimension ref="A1:Q31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12:M12"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.15"/>
@@ -4525,11 +4535,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -5283,7 +5293,7 @@
       <c r="E20" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="28" t="s">
+      <c r="F20" s="58" t="s">
         <v>244</v>
       </c>
       <c r="H20" s="28" t="s">
@@ -5618,11 +5628,11 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="O7" s="56" t="s">
+      <c r="O7" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="P7" s="56"/>
-      <c r="Q7" s="56"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
     </row>
     <row r="8" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -8082,7 +8092,7 @@
       <c r="A60" s="36">
         <v>107</v>
       </c>
-      <c r="B60" s="57" t="s">
+      <c r="B60" s="56" t="s">
         <v>457</v>
       </c>
       <c r="J60" s="36">
@@ -8106,7 +8116,7 @@
       <c r="A61" s="36">
         <v>108</v>
       </c>
-      <c r="B61" s="57" t="s">
+      <c r="B61" s="56" t="s">
         <v>458</v>
       </c>
       <c r="J61" s="36">
@@ -8130,7 +8140,7 @@
       <c r="A62" s="36">
         <v>109</v>
       </c>
-      <c r="B62" s="57" t="s">
+      <c r="B62" s="56" t="s">
         <v>459</v>
       </c>
       <c r="J62" s="36">
@@ -8204,11 +8214,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="56" t="s">
+      <c r="O3" s="57" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="56"/>
-      <c r="Q3" s="56"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>

</xml_diff>

<commit_message>
BOM update to show assembled components so far
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A806B6-63DC-764E-A98F-9E45F6DDFCDC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DFEEAF-6D3D-DF48-A145-1E3A21B9A3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2440" windowWidth="37640" windowHeight="20000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5980" yWindow="3120" windowWidth="32420" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept Estimate" sheetId="1" r:id="rId1"/>
@@ -1607,7 +1607,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1733,11 +1733,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4493,7 +4502,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F5DBFB5-E21A-7B4B-815F-748A526FD280}">
   <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
+    <sheetView topLeftCell="A9" zoomScale="125" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -4535,11 +4544,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="57" t="s">
+      <c r="O3" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -5293,7 +5302,7 @@
       <c r="E20" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="58" t="s">
+      <c r="F20" s="57" t="s">
         <v>244</v>
       </c>
       <c r="H20" s="28" t="s">
@@ -5559,15 +5568,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView topLeftCell="A27" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B44" sqref="B44:F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="36"/>
     <col min="2" max="2" width="40.6640625" style="36" customWidth="1"/>
-    <col min="3" max="3" width="27" style="37" customWidth="1"/>
+    <col min="3" max="3" width="55" style="37" customWidth="1"/>
     <col min="4" max="4" width="10.83203125" style="36"/>
     <col min="5" max="5" width="5.83203125" style="28" customWidth="1"/>
     <col min="6" max="7" width="27" style="37" customWidth="1"/>
@@ -5628,11 +5637,11 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="O7" s="57" t="s">
+      <c r="O7" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="P7" s="57"/>
-      <c r="Q7" s="57"/>
+      <c r="P7" s="61"/>
+      <c r="Q7" s="61"/>
     </row>
     <row r="8" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -5953,19 +5962,19 @@
       <c r="A14" s="36">
         <v>4</v>
       </c>
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="58" t="s">
         <v>292</v>
       </c>
-      <c r="C14" s="36" t="s">
+      <c r="C14" s="59" t="s">
         <v>293</v>
       </c>
-      <c r="D14" s="38">
-        <v>1</v>
-      </c>
-      <c r="E14" s="28" t="s">
+      <c r="D14" s="60">
+        <v>1</v>
+      </c>
+      <c r="E14" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F14" s="36" t="s">
+      <c r="F14" s="59" t="s">
         <v>294</v>
       </c>
       <c r="G14" s="36" t="s">
@@ -6132,19 +6141,19 @@
       <c r="A17" s="36">
         <v>7</v>
       </c>
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="58" t="s">
         <v>306</v>
       </c>
-      <c r="C17" s="36" t="s">
+      <c r="C17" s="59" t="s">
         <v>307</v>
       </c>
-      <c r="D17" s="38">
-        <v>1</v>
-      </c>
-      <c r="E17" s="28" t="s">
+      <c r="D17" s="60">
+        <v>1</v>
+      </c>
+      <c r="E17" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F17" s="36" t="s">
+      <c r="F17" s="59" t="s">
         <v>308</v>
       </c>
       <c r="G17" s="36" t="s">
@@ -6232,19 +6241,19 @@
       <c r="A20" s="36">
         <v>10</v>
       </c>
-      <c r="B20" s="37" t="s">
+      <c r="B20" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="C20" s="36" t="s">
+      <c r="C20" s="59" t="s">
         <v>311</v>
       </c>
-      <c r="D20" s="38">
-        <v>1</v>
-      </c>
-      <c r="E20" s="28" t="s">
+      <c r="D20" s="60">
+        <v>1</v>
+      </c>
+      <c r="E20" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="59" t="s">
         <v>312</v>
       </c>
       <c r="G20" s="36" t="s">
@@ -6440,7 +6449,7 @@
         <f>IF(I23&gt;D23,0,D23-I23)</f>
         <v>1</v>
       </c>
-      <c r="K23" s="28">
+      <c r="K23" s="30">
         <f>I23+J23</f>
         <v>1</v>
       </c>
@@ -6630,19 +6639,19 @@
       <c r="A31" s="36">
         <v>21</v>
       </c>
-      <c r="B31" s="37" t="s">
+      <c r="B31" s="58" t="s">
         <v>339</v>
       </c>
-      <c r="C31" s="36" t="s">
+      <c r="C31" s="59" t="s">
         <v>340</v>
       </c>
-      <c r="D31" s="38">
-        <v>1</v>
-      </c>
-      <c r="E31" s="28" t="s">
+      <c r="D31" s="60">
+        <v>1</v>
+      </c>
+      <c r="E31" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="59" t="s">
         <v>341</v>
       </c>
       <c r="G31" s="36" t="s">
@@ -6832,20 +6841,20 @@
       <c r="A34" s="36">
         <v>24</v>
       </c>
-      <c r="B34" s="37" t="s">
+      <c r="B34" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="C34" s="36" t="s">
+      <c r="C34" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="D34" s="38">
-        <v>1</v>
-      </c>
-      <c r="E34" s="28" t="s">
+      <c r="D34" s="60">
+        <v>1</v>
+      </c>
+      <c r="E34" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F34" s="36">
-        <v>1E-3</v>
+      <c r="F34" s="59">
+        <v>0.1</v>
       </c>
       <c r="G34" s="36"/>
       <c r="H34" s="36" t="s">
@@ -7291,19 +7300,19 @@
       <c r="A43" s="36">
         <v>33</v>
       </c>
-      <c r="B43" s="37" t="s">
+      <c r="B43" s="58" t="s">
         <v>375</v>
       </c>
-      <c r="C43" s="36" t="s">
+      <c r="C43" s="59" t="s">
         <v>376</v>
       </c>
-      <c r="D43" s="38">
-        <v>1</v>
-      </c>
-      <c r="E43" s="28" t="s">
+      <c r="D43" s="60">
+        <v>1</v>
+      </c>
+      <c r="E43" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F43" s="36" t="s">
+      <c r="F43" s="59" t="s">
         <v>377</v>
       </c>
       <c r="G43" s="36" t="s">
@@ -7343,19 +7352,19 @@
       <c r="A44" s="36">
         <v>34</v>
       </c>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="58" t="s">
         <v>235</v>
       </c>
-      <c r="C44" s="36" t="s">
+      <c r="C44" s="59" t="s">
         <v>380</v>
       </c>
-      <c r="D44" s="38">
-        <v>1</v>
-      </c>
-      <c r="E44" s="28" t="s">
+      <c r="D44" s="60">
+        <v>1</v>
+      </c>
+      <c r="E44" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F44" s="36" t="s">
+      <c r="F44" s="59" t="s">
         <v>381</v>
       </c>
       <c r="G44" s="36" t="s">
@@ -7702,19 +7711,19 @@
       <c r="A51" s="36">
         <v>41</v>
       </c>
-      <c r="B51" s="37" t="s">
+      <c r="B51" s="58" t="s">
         <v>251</v>
       </c>
-      <c r="C51" s="36" t="s">
+      <c r="C51" s="59" t="s">
         <v>414</v>
       </c>
-      <c r="D51" s="38">
-        <v>1</v>
-      </c>
-      <c r="E51" s="28" t="s">
+      <c r="D51" s="60">
+        <v>1</v>
+      </c>
+      <c r="E51" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F51" s="36" t="s">
+      <c r="F51" s="59" t="s">
         <v>415</v>
       </c>
       <c r="G51" s="37" t="s">
@@ -7806,19 +7815,19 @@
       <c r="A53" s="36">
         <v>43</v>
       </c>
-      <c r="B53" s="37" t="s">
+      <c r="B53" s="58" t="s">
         <v>423</v>
       </c>
-      <c r="C53" s="36" t="s">
+      <c r="C53" s="59" t="s">
         <v>424</v>
       </c>
-      <c r="D53" s="38">
-        <v>1</v>
-      </c>
-      <c r="E53" s="28" t="s">
+      <c r="D53" s="60">
+        <v>1</v>
+      </c>
+      <c r="E53" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F53" s="36" t="s">
+      <c r="F53" s="59" t="s">
         <v>425</v>
       </c>
       <c r="G53" s="36"/>
@@ -8036,13 +8045,14 @@
       <c r="A58" s="36">
         <v>105</v>
       </c>
-      <c r="B58" s="36" t="s">
+      <c r="B58" s="59" t="s">
         <v>142</v>
       </c>
-      <c r="D58" s="38">
-        <v>1</v>
-      </c>
-      <c r="E58" s="28" t="s">
+      <c r="C58" s="58"/>
+      <c r="D58" s="60">
+        <v>1</v>
+      </c>
+      <c r="E58" s="30" t="s">
         <v>203</v>
       </c>
       <c r="G58" s="37" t="s">
@@ -8214,11 +8224,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="57" t="s">
+      <c r="O3" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="57"/>
-      <c r="Q3" s="57"/>
+      <c r="P3" s="61"/>
+      <c r="Q3" s="61"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>

</xml_diff>

<commit_message>
Add Teensy LC cut Vin-Vusb instructions, BOM assembly tracking Board ID section.
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74DFEEAF-6D3D-DF48-A145-1E3A21B9A3AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AA766C-348B-2545-AACE-ACACC642827F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5980" yWindow="3120" windowWidth="32420" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3640" yWindow="2160" windowWidth="32420" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept Estimate" sheetId="1" r:id="rId1"/>
@@ -5568,8 +5568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B44" sqref="B44:F44"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C35" sqref="C34:F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5851,7 +5851,7 @@
       <c r="A12" s="36">
         <v>2</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="58" t="s">
         <v>287</v>
       </c>
       <c r="C12" s="36" t="s">
@@ -6891,19 +6891,19 @@
       <c r="A35" s="36">
         <v>25</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="58" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="59" t="s">
         <v>358</v>
       </c>
-      <c r="D35" s="38">
+      <c r="D35" s="60">
         <v>2</v>
       </c>
-      <c r="E35" s="28" t="s">
+      <c r="E35" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F35" s="36" t="s">
+      <c r="F35" s="59" t="s">
         <v>234</v>
       </c>
       <c r="G35" s="36" t="s">
@@ -7248,7 +7248,7 @@
       <c r="A42" s="36">
         <v>32</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="58" t="s">
         <v>373</v>
       </c>
       <c r="C42" s="36" t="s">
@@ -7404,19 +7404,19 @@
       <c r="A45" s="36">
         <v>35</v>
       </c>
-      <c r="B45" s="37" t="s">
+      <c r="B45" s="58" t="s">
         <v>385</v>
       </c>
-      <c r="C45" s="36" t="s">
+      <c r="C45" s="59" t="s">
         <v>386</v>
       </c>
-      <c r="D45" s="38">
-        <v>1</v>
-      </c>
-      <c r="E45" s="28" t="s">
+      <c r="D45" s="60">
+        <v>1</v>
+      </c>
+      <c r="E45" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F45" s="36" t="s">
+      <c r="F45" s="59" t="s">
         <v>137</v>
       </c>
       <c r="G45" s="36"/>
@@ -7451,19 +7451,19 @@
       <c r="A46" s="36">
         <v>36</v>
       </c>
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="C46" s="36" t="s">
+      <c r="C46" s="59" t="s">
         <v>388</v>
       </c>
-      <c r="D46" s="38">
-        <v>1</v>
-      </c>
-      <c r="E46" s="28" t="s">
+      <c r="D46" s="60">
+        <v>1</v>
+      </c>
+      <c r="E46" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F46" s="36" t="s">
+      <c r="F46" s="59" t="s">
         <v>389</v>
       </c>
       <c r="G46" s="36" t="s">
@@ -7555,7 +7555,7 @@
       <c r="A48" s="36">
         <v>38</v>
       </c>
-      <c r="B48" s="37" t="s">
+      <c r="B48" s="58" t="s">
         <v>399</v>
       </c>
       <c r="C48" s="36" t="s">
@@ -7763,7 +7763,7 @@
       <c r="A52" s="36">
         <v>42</v>
       </c>
-      <c r="B52" s="37" t="s">
+      <c r="B52" s="58" t="s">
         <v>418</v>
       </c>
       <c r="C52" s="36" t="s">
@@ -7996,7 +7996,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="57" spans="1:19" ht="34" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:19" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="36">
         <v>104</v>
       </c>

</xml_diff>

<commit_message>
Hardware detection working. Removed src/libraries conflicts to rely on Arduino Library Manager.
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3AA766C-348B-2545-AACE-ACACC642827F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2531B7-9242-0846-94CE-CE5930F9F91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3640" yWindow="2160" windowWidth="32420" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5568,8 +5568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C35" sqref="C34:F35"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7424,7 +7424,7 @@
         <v>206</v>
       </c>
       <c r="I45" s="36">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45" s="28">
         <f t="shared" si="7"/>
@@ -7432,15 +7432,15 @@
       </c>
       <c r="K45" s="28">
         <f t="shared" si="4"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L45" s="28">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M45" s="28">
         <f t="shared" si="6"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="N45" s="28"/>
       <c r="R45" s="36" t="s">

</xml_diff>

<commit_message>
LED Array works with TopLevelState = STATE_LED_TEST_ONE_MATRIX_COLOR !
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C2531B7-9242-0846-94CE-CE5930F9F91F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F29E46-7892-AF42-8283-A7924672B644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3640" yWindow="2160" windowWidth="32420" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3620" yWindow="2160" windowWidth="32420" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept Estimate" sheetId="1" r:id="rId1"/>
@@ -927,9 +927,6 @@
     <t>Diode_SMD:D_SOD-123F</t>
   </si>
   <si>
-    <t>MBR120</t>
-  </si>
-  <si>
     <t>MBR120VLSFT1GOSCT-ND</t>
   </si>
   <si>
@@ -1423,6 +1420,9 @@
   </si>
   <si>
     <t>Solder paste, Syringe Tip</t>
+  </si>
+  <si>
+    <t>MBR120 CHANGE?? S1M-13-F</t>
   </si>
 </sst>
 </file>
@@ -1434,10 +1434,17 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1504,7 +1511,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1526,6 +1533,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1603,36 +1616,36 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1642,111 +1655,123 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -5568,8 +5593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5703,7 +5728,7 @@
     </row>
     <row r="10" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="36" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B10" s="37" t="s">
         <v>189</v>
@@ -5974,11 +5999,11 @@
       <c r="E14" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F14" s="59" t="s">
+      <c r="F14" s="62" t="s">
+        <v>459</v>
+      </c>
+      <c r="G14" s="63" t="s">
         <v>294</v>
-      </c>
-      <c r="G14" s="36" t="s">
-        <v>295</v>
       </c>
       <c r="H14" s="36" t="s">
         <v>206</v>
@@ -6011,10 +6036,10 @@
         <v>0</v>
       </c>
       <c r="R14" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="S14" s="36" t="s">
         <v>296</v>
-      </c>
-      <c r="S14" s="36" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:30" ht="17" x14ac:dyDescent="0.2">
@@ -6022,10 +6047,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="37" t="s">
+        <v>297</v>
+      </c>
+      <c r="C15" s="36" t="s">
         <v>298</v>
-      </c>
-      <c r="C15" s="36" t="s">
-        <v>299</v>
       </c>
       <c r="D15" s="38">
         <v>6</v>
@@ -6034,7 +6059,7 @@
         <v>203</v>
       </c>
       <c r="F15" s="36" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="G15" s="36" t="s">
         <v>103</v>
@@ -6071,10 +6096,10 @@
         <v>0</v>
       </c>
       <c r="R15" s="36" t="s">
+        <v>300</v>
+      </c>
+      <c r="S15" s="36" t="s">
         <v>301</v>
-      </c>
-      <c r="S15" s="36" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="16" spans="1:30" ht="17" x14ac:dyDescent="0.2">
@@ -6082,10 +6107,10 @@
         <v>6</v>
       </c>
       <c r="B16" s="37" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C16" s="36" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D16" s="38">
         <v>6</v>
@@ -6094,7 +6119,7 @@
         <v>203</v>
       </c>
       <c r="F16" s="36" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="G16" s="37" t="s">
         <v>109</v>
@@ -6131,10 +6156,10 @@
         <v>0</v>
       </c>
       <c r="R16" s="36" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="S16" s="36" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:30" ht="17" x14ac:dyDescent="0.2">
@@ -6142,10 +6167,10 @@
         <v>7</v>
       </c>
       <c r="B17" s="58" t="s">
+        <v>305</v>
+      </c>
+      <c r="C17" s="59" t="s">
         <v>306</v>
-      </c>
-      <c r="C17" s="59" t="s">
-        <v>307</v>
       </c>
       <c r="D17" s="60">
         <v>1</v>
@@ -6154,7 +6179,7 @@
         <v>203</v>
       </c>
       <c r="F17" s="59" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="G17" s="36" t="s">
         <v>30</v>
@@ -6187,7 +6212,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R17" s="36" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="S17" s="36" t="s">
         <v>286</v>
@@ -6242,10 +6267,10 @@
         <v>10</v>
       </c>
       <c r="B20" s="58" t="s">
+        <v>309</v>
+      </c>
+      <c r="C20" s="59" t="s">
         <v>310</v>
-      </c>
-      <c r="C20" s="59" t="s">
-        <v>311</v>
       </c>
       <c r="D20" s="60">
         <v>1</v>
@@ -6253,11 +6278,11 @@
       <c r="E20" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="59" t="s">
+      <c r="F20" s="63" t="s">
+        <v>311</v>
+      </c>
+      <c r="G20" s="63" t="s">
         <v>312</v>
-      </c>
-      <c r="G20" s="36" t="s">
-        <v>313</v>
       </c>
       <c r="H20" s="36" t="s">
         <v>206</v>
@@ -6287,45 +6312,45 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R20" s="36" t="s">
+        <v>313</v>
+      </c>
+      <c r="S20" s="36" t="s">
         <v>314</v>
       </c>
-      <c r="S20" s="36" t="s">
+      <c r="W20" s="36" t="s">
         <v>315</v>
-      </c>
-      <c r="W20" s="36" t="s">
-        <v>316</v>
       </c>
       <c r="Y20" s="36">
         <v>8.8000000000000007</v>
       </c>
       <c r="AB20" s="36" t="s">
+        <v>316</v>
+      </c>
+      <c r="AC20" s="36" t="s">
         <v>317</v>
-      </c>
-      <c r="AC20" s="36" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="21" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="36">
         <v>11</v>
       </c>
-      <c r="B21" s="37" t="s">
+      <c r="B21" s="64" t="s">
+        <v>318</v>
+      </c>
+      <c r="C21" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="C21" s="36" t="s">
+      <c r="D21" s="65">
+        <v>1</v>
+      </c>
+      <c r="E21" s="40" t="s">
+        <v>203</v>
+      </c>
+      <c r="F21" s="39" t="s">
         <v>320</v>
       </c>
-      <c r="D21" s="38">
-        <v>1</v>
-      </c>
-      <c r="E21" s="28" t="s">
-        <v>203</v>
-      </c>
-      <c r="F21" s="36" t="s">
+      <c r="G21" s="39" t="s">
         <v>321</v>
-      </c>
-      <c r="G21" s="36" t="s">
-        <v>322</v>
       </c>
       <c r="H21" s="36" t="s">
         <v>229</v>
@@ -6355,7 +6380,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R21" s="36" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="S21" s="36" t="s">
         <v>286</v>
@@ -6365,11 +6390,11 @@
       <c r="A22" s="36">
         <v>12</v>
       </c>
-      <c r="B22" s="37" t="s">
+      <c r="B22" s="58" t="s">
+        <v>323</v>
+      </c>
+      <c r="C22" s="36" t="s">
         <v>324</v>
-      </c>
-      <c r="C22" s="36" t="s">
-        <v>325</v>
       </c>
       <c r="D22" s="38">
         <v>4</v>
@@ -6378,10 +6403,10 @@
         <v>203</v>
       </c>
       <c r="F22" s="36" t="s">
+        <v>325</v>
+      </c>
+      <c r="G22" s="36" t="s">
         <v>326</v>
-      </c>
-      <c r="G22" s="36" t="s">
-        <v>327</v>
       </c>
       <c r="H22" s="36" t="s">
         <v>229</v>
@@ -6411,7 +6436,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R22" s="36" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="S22" s="36" t="s">
         <v>286</v>
@@ -6422,10 +6447,10 @@
         <v>13</v>
       </c>
       <c r="B23" s="37" t="s">
+        <v>328</v>
+      </c>
+      <c r="C23" s="36" t="s">
         <v>329</v>
-      </c>
-      <c r="C23" s="36" t="s">
-        <v>330</v>
       </c>
       <c r="D23" s="38">
         <v>1</v>
@@ -6434,10 +6459,10 @@
         <v>203</v>
       </c>
       <c r="F23" s="36" t="s">
+        <v>330</v>
+      </c>
+      <c r="G23" s="37" t="s">
         <v>331</v>
-      </c>
-      <c r="G23" s="37" t="s">
-        <v>332</v>
       </c>
       <c r="H23" s="36" t="s">
         <v>229</v>
@@ -6467,7 +6492,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R23" s="36" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="S23" s="36" t="s">
         <v>286</v>
@@ -6478,10 +6503,10 @@
         <v>14</v>
       </c>
       <c r="B24" s="37" t="s">
+        <v>333</v>
+      </c>
+      <c r="C24" s="36" t="s">
         <v>334</v>
-      </c>
-      <c r="C24" s="36" t="s">
-        <v>335</v>
       </c>
       <c r="D24" s="38">
         <v>2</v>
@@ -6490,10 +6515,10 @@
         <v>203</v>
       </c>
       <c r="F24" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="G24" s="36" t="s">
         <v>336</v>
-      </c>
-      <c r="G24" s="36" t="s">
-        <v>337</v>
       </c>
       <c r="H24" s="36" t="s">
         <v>206</v>
@@ -6523,7 +6548,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="R24" s="36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S24" s="36" t="s">
         <v>286</v>
@@ -6640,10 +6665,10 @@
         <v>21</v>
       </c>
       <c r="B31" s="58" t="s">
+        <v>338</v>
+      </c>
+      <c r="C31" s="59" t="s">
         <v>339</v>
-      </c>
-      <c r="C31" s="59" t="s">
-        <v>340</v>
       </c>
       <c r="D31" s="60">
         <v>1</v>
@@ -6652,10 +6677,10 @@
         <v>203</v>
       </c>
       <c r="F31" s="59" t="s">
+        <v>340</v>
+      </c>
+      <c r="G31" s="36" t="s">
         <v>341</v>
-      </c>
-      <c r="G31" s="36" t="s">
-        <v>342</v>
       </c>
       <c r="H31" s="36" t="s">
         <v>206</v>
@@ -6681,10 +6706,10 @@
       </c>
       <c r="N31" s="28"/>
       <c r="R31" s="36" t="s">
+        <v>342</v>
+      </c>
+      <c r="S31" s="36" t="s">
         <v>343</v>
-      </c>
-      <c r="S31" s="36" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="32" spans="1:30" ht="17" x14ac:dyDescent="0.2">
@@ -6692,10 +6717,10 @@
         <v>22</v>
       </c>
       <c r="B32" s="37" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="C32" s="36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D32" s="38">
         <v>10</v>
@@ -6732,34 +6757,34 @@
       </c>
       <c r="N32" s="28"/>
       <c r="R32" s="36" t="s">
+        <v>345</v>
+      </c>
+      <c r="S32" s="36" t="s">
         <v>346</v>
       </c>
-      <c r="S32" s="36" t="s">
+      <c r="T32" s="36" t="s">
         <v>347</v>
       </c>
-      <c r="T32" s="36" t="s">
+      <c r="U32" s="36" t="s">
+        <v>346</v>
+      </c>
+      <c r="V32" s="36" t="s">
         <v>348</v>
-      </c>
-      <c r="U32" s="36" t="s">
-        <v>347</v>
-      </c>
-      <c r="V32" s="36" t="s">
-        <v>349</v>
       </c>
       <c r="W32" s="36" t="s">
         <v>8</v>
       </c>
       <c r="X32" s="36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z32" s="36" t="s">
         <v>7</v>
       </c>
       <c r="AA32" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="AD32" s="36" t="s">
         <v>351</v>
-      </c>
-      <c r="AD32" s="36" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="33" spans="1:30" ht="34" x14ac:dyDescent="0.2">
@@ -6767,10 +6792,10 @@
         <v>23</v>
       </c>
       <c r="B33" s="37" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C33" s="36" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D33" s="38">
         <v>11</v>
@@ -6807,34 +6832,34 @@
       </c>
       <c r="N33" s="28"/>
       <c r="R33" s="36" t="s">
+        <v>353</v>
+      </c>
+      <c r="S33" s="36" t="s">
         <v>354</v>
       </c>
-      <c r="S33" s="36" t="s">
+      <c r="T33" s="36" t="s">
+        <v>347</v>
+      </c>
+      <c r="U33" s="36" t="s">
+        <v>354</v>
+      </c>
+      <c r="V33" s="36" t="s">
         <v>355</v>
-      </c>
-      <c r="T33" s="36" t="s">
-        <v>348</v>
-      </c>
-      <c r="U33" s="36" t="s">
-        <v>355</v>
-      </c>
-      <c r="V33" s="36" t="s">
-        <v>356</v>
       </c>
       <c r="W33" s="36" t="s">
         <v>14</v>
       </c>
       <c r="X33" s="36" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="Z33" s="36" t="s">
         <v>13</v>
       </c>
       <c r="AA33" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="AD33" s="36" t="s">
         <v>351</v>
-      </c>
-      <c r="AD33" s="36" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="34" spans="1:30" ht="17" x14ac:dyDescent="0.2">
@@ -6842,10 +6867,10 @@
         <v>24</v>
       </c>
       <c r="B34" s="58" t="s">
+        <v>356</v>
+      </c>
+      <c r="C34" s="59" t="s">
         <v>357</v>
-      </c>
-      <c r="C34" s="59" t="s">
-        <v>358</v>
       </c>
       <c r="D34" s="60">
         <v>1</v>
@@ -6881,7 +6906,7 @@
       </c>
       <c r="N34" s="28"/>
       <c r="R34" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S34" s="36" t="s">
         <v>286</v>
@@ -6892,10 +6917,10 @@
         <v>25</v>
       </c>
       <c r="B35" s="58" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C35" s="59" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D35" s="60">
         <v>2</v>
@@ -6932,7 +6957,7 @@
       </c>
       <c r="N35" s="28"/>
       <c r="R35" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S35" s="36" t="s">
         <v>286</v>
@@ -6942,11 +6967,11 @@
       <c r="A36" s="36">
         <v>26</v>
       </c>
-      <c r="B36" s="37" t="s">
-        <v>361</v>
+      <c r="B36" s="58" t="s">
+        <v>360</v>
       </c>
       <c r="C36" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D36" s="38">
         <v>1</v>
@@ -6958,7 +6983,7 @@
         <v>300</v>
       </c>
       <c r="G36" s="39" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H36" s="36" t="s">
         <v>206</v>
@@ -6981,7 +7006,7 @@
       </c>
       <c r="N36" s="28"/>
       <c r="R36" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S36" s="36" t="s">
         <v>286</v>
@@ -6992,10 +7017,10 @@
         <v>27</v>
       </c>
       <c r="B37" s="37" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="C37" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D37" s="38">
         <v>21</v>
@@ -7007,7 +7032,7 @@
         <v>470</v>
       </c>
       <c r="G37" s="36" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H37" s="36" t="s">
         <v>206</v>
@@ -7032,7 +7057,7 @@
       </c>
       <c r="N37" s="28"/>
       <c r="R37" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S37" s="36" t="s">
         <v>286</v>
@@ -7043,10 +7068,10 @@
         <v>28</v>
       </c>
       <c r="B38" s="37" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="C38" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D38" s="38">
         <v>6</v>
@@ -7055,7 +7080,7 @@
         <v>203</v>
       </c>
       <c r="F38" s="36" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="G38" s="36" t="s">
         <v>65</v>
@@ -7083,7 +7108,7 @@
       </c>
       <c r="N38" s="28"/>
       <c r="R38" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S38" s="36" t="s">
         <v>286</v>
@@ -7094,10 +7119,10 @@
         <v>29</v>
       </c>
       <c r="B39" s="37" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="C39" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D39" s="38">
         <v>3</v>
@@ -7106,7 +7131,7 @@
         <v>203</v>
       </c>
       <c r="F39" s="36" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="G39" s="36" t="s">
         <v>89</v>
@@ -7135,7 +7160,7 @@
       </c>
       <c r="N39" s="28"/>
       <c r="R39" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S39" s="36" t="s">
         <v>286</v>
@@ -7146,10 +7171,10 @@
         <v>30</v>
       </c>
       <c r="B40" s="37" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C40" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D40" s="38">
         <v>2</v>
@@ -7158,7 +7183,7 @@
         <v>203</v>
       </c>
       <c r="F40" s="36" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="G40" s="36" t="s">
         <v>94</v>
@@ -7187,7 +7212,7 @@
       </c>
       <c r="N40" s="28"/>
       <c r="R40" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S40" s="36" t="s">
         <v>286</v>
@@ -7198,10 +7223,10 @@
         <v>31</v>
       </c>
       <c r="B41" s="37" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C41" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D41" s="38">
         <v>2</v>
@@ -7213,7 +7238,7 @@
         <v>11</v>
       </c>
       <c r="G41" s="36" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H41" s="36" t="s">
         <v>206</v>
@@ -7238,7 +7263,7 @@
       </c>
       <c r="N41" s="28"/>
       <c r="R41" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S41" s="36" t="s">
         <v>286</v>
@@ -7249,10 +7274,10 @@
         <v>32</v>
       </c>
       <c r="B42" s="58" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C42" s="36" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="D42" s="38">
         <v>6</v>
@@ -7261,7 +7286,7 @@
         <v>203</v>
       </c>
       <c r="F42" s="36" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="G42" s="36" t="s">
         <v>82</v>
@@ -7290,7 +7315,7 @@
       </c>
       <c r="N42" s="28"/>
       <c r="R42" s="36" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="S42" s="36" t="s">
         <v>286</v>
@@ -7301,10 +7326,10 @@
         <v>33</v>
       </c>
       <c r="B43" s="58" t="s">
+        <v>374</v>
+      </c>
+      <c r="C43" s="59" t="s">
         <v>375</v>
-      </c>
-      <c r="C43" s="59" t="s">
-        <v>376</v>
       </c>
       <c r="D43" s="60">
         <v>1</v>
@@ -7313,10 +7338,10 @@
         <v>203</v>
       </c>
       <c r="F43" s="59" t="s">
+        <v>376</v>
+      </c>
+      <c r="G43" s="36" t="s">
         <v>377</v>
-      </c>
-      <c r="G43" s="36" t="s">
-        <v>378</v>
       </c>
       <c r="H43" s="36" t="s">
         <v>206</v>
@@ -7342,7 +7367,7 @@
       </c>
       <c r="N43" s="28"/>
       <c r="R43" s="36" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="S43" s="36" t="s">
         <v>286</v>
@@ -7356,7 +7381,7 @@
         <v>235</v>
       </c>
       <c r="C44" s="59" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D44" s="60">
         <v>1</v>
@@ -7365,10 +7390,10 @@
         <v>203</v>
       </c>
       <c r="F44" s="59" t="s">
+        <v>380</v>
+      </c>
+      <c r="G44" s="36" t="s">
         <v>381</v>
-      </c>
-      <c r="G44" s="36" t="s">
-        <v>382</v>
       </c>
       <c r="H44" s="36" t="s">
         <v>206</v>
@@ -7394,10 +7419,10 @@
       </c>
       <c r="N44" s="28"/>
       <c r="R44" s="36" t="s">
+        <v>382</v>
+      </c>
+      <c r="S44" s="36" t="s">
         <v>383</v>
-      </c>
-      <c r="S44" s="36" t="s">
-        <v>384</v>
       </c>
     </row>
     <row r="45" spans="1:30" ht="17" x14ac:dyDescent="0.2">
@@ -7405,10 +7430,10 @@
         <v>35</v>
       </c>
       <c r="B45" s="58" t="s">
+        <v>384</v>
+      </c>
+      <c r="C45" s="59" t="s">
         <v>385</v>
-      </c>
-      <c r="C45" s="59" t="s">
-        <v>386</v>
       </c>
       <c r="D45" s="60">
         <v>1</v>
@@ -7444,7 +7469,7 @@
       </c>
       <c r="N45" s="28"/>
       <c r="R45" s="36" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="46" spans="1:30" ht="17" x14ac:dyDescent="0.2">
@@ -7455,7 +7480,7 @@
         <v>240</v>
       </c>
       <c r="C46" s="59" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D46" s="60">
         <v>1</v>
@@ -7464,10 +7489,10 @@
         <v>203</v>
       </c>
       <c r="F46" s="59" t="s">
+        <v>388</v>
+      </c>
+      <c r="G46" s="36" t="s">
         <v>389</v>
-      </c>
-      <c r="G46" s="36" t="s">
-        <v>390</v>
       </c>
       <c r="H46" s="36" t="s">
         <v>206</v>
@@ -7493,21 +7518,21 @@
       </c>
       <c r="N46" s="28"/>
       <c r="R46" s="36" t="s">
+        <v>390</v>
+      </c>
+      <c r="S46" s="36" t="s">
         <v>391</v>
-      </c>
-      <c r="S46" s="36" t="s">
-        <v>392</v>
       </c>
     </row>
     <row r="47" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="36">
         <v>37</v>
       </c>
-      <c r="B47" s="37" t="s">
+      <c r="B47" s="58" t="s">
+        <v>392</v>
+      </c>
+      <c r="C47" s="36" t="s">
         <v>393</v>
-      </c>
-      <c r="C47" s="36" t="s">
-        <v>394</v>
       </c>
       <c r="D47" s="38">
         <v>1</v>
@@ -7516,10 +7541,10 @@
         <v>203</v>
       </c>
       <c r="F47" s="36" t="s">
+        <v>394</v>
+      </c>
+      <c r="G47" s="36" t="s">
         <v>395</v>
-      </c>
-      <c r="G47" s="36" t="s">
-        <v>396</v>
       </c>
       <c r="H47" s="36" t="s">
         <v>206</v>
@@ -7545,10 +7570,10 @@
       </c>
       <c r="N47" s="28"/>
       <c r="R47" s="36" t="s">
+        <v>396</v>
+      </c>
+      <c r="S47" s="36" t="s">
         <v>397</v>
-      </c>
-      <c r="S47" s="36" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="48" spans="1:30" ht="17" x14ac:dyDescent="0.2">
@@ -7556,10 +7581,10 @@
         <v>38</v>
       </c>
       <c r="B48" s="58" t="s">
+        <v>398</v>
+      </c>
+      <c r="C48" s="36" t="s">
         <v>399</v>
-      </c>
-      <c r="C48" s="36" t="s">
-        <v>400</v>
       </c>
       <c r="D48" s="38">
         <v>2</v>
@@ -7568,10 +7593,10 @@
         <v>203</v>
       </c>
       <c r="F48" s="36" t="s">
+        <v>400</v>
+      </c>
+      <c r="G48" s="36" t="s">
         <v>401</v>
-      </c>
-      <c r="G48" s="36" t="s">
-        <v>402</v>
       </c>
       <c r="H48" s="36" t="s">
         <v>206</v>
@@ -7597,10 +7622,10 @@
       </c>
       <c r="N48" s="28"/>
       <c r="R48" s="36" t="s">
+        <v>402</v>
+      </c>
+      <c r="S48" s="36" t="s">
         <v>403</v>
-      </c>
-      <c r="S48" s="36" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="49" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -7611,7 +7636,7 @@
         <v>247</v>
       </c>
       <c r="C49" s="36" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D49" s="38">
         <v>1</v>
@@ -7620,7 +7645,7 @@
         <v>203</v>
       </c>
       <c r="F49" s="36" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="G49" s="36" t="s">
         <v>17</v>
@@ -7649,10 +7674,10 @@
       </c>
       <c r="N49" s="28"/>
       <c r="R49" s="36" t="s">
+        <v>406</v>
+      </c>
+      <c r="S49" s="36" t="s">
         <v>407</v>
-      </c>
-      <c r="S49" s="36" t="s">
-        <v>408</v>
       </c>
     </row>
     <row r="50" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -7663,7 +7688,7 @@
         <v>249</v>
       </c>
       <c r="C50" s="36" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D50" s="38">
         <v>1</v>
@@ -7672,10 +7697,10 @@
         <v>203</v>
       </c>
       <c r="F50" s="36" t="s">
+        <v>409</v>
+      </c>
+      <c r="G50" s="36" t="s">
         <v>410</v>
-      </c>
-      <c r="G50" s="36" t="s">
-        <v>411</v>
       </c>
       <c r="H50" s="36" t="s">
         <v>206</v>
@@ -7701,10 +7726,10 @@
       </c>
       <c r="N50" s="28"/>
       <c r="R50" s="36" t="s">
+        <v>411</v>
+      </c>
+      <c r="S50" s="36" t="s">
         <v>412</v>
-      </c>
-      <c r="S50" s="36" t="s">
-        <v>413</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="17" x14ac:dyDescent="0.2">
@@ -7715,7 +7740,7 @@
         <v>251</v>
       </c>
       <c r="C51" s="59" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D51" s="60">
         <v>1</v>
@@ -7724,10 +7749,10 @@
         <v>203</v>
       </c>
       <c r="F51" s="59" t="s">
+        <v>414</v>
+      </c>
+      <c r="G51" s="37" t="s">
         <v>415</v>
-      </c>
-      <c r="G51" s="37" t="s">
-        <v>416</v>
       </c>
       <c r="H51" s="36" t="s">
         <v>229</v>
@@ -7753,7 +7778,7 @@
       </c>
       <c r="N51" s="28"/>
       <c r="R51" s="36" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="S51" s="36" t="s">
         <v>286</v>
@@ -7764,10 +7789,10 @@
         <v>42</v>
       </c>
       <c r="B52" s="58" t="s">
+        <v>417</v>
+      </c>
+      <c r="C52" s="36" t="s">
         <v>418</v>
-      </c>
-      <c r="C52" s="36" t="s">
-        <v>419</v>
       </c>
       <c r="D52" s="38">
         <v>1</v>
@@ -7776,10 +7801,10 @@
         <v>203</v>
       </c>
       <c r="F52" s="36" t="s">
+        <v>419</v>
+      </c>
+      <c r="G52" s="36" t="s">
         <v>420</v>
-      </c>
-      <c r="G52" s="36" t="s">
-        <v>421</v>
       </c>
       <c r="H52" s="36" t="s">
         <v>229</v>
@@ -7805,7 +7830,7 @@
       </c>
       <c r="N52" s="28"/>
       <c r="R52" s="36" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="S52" s="36" t="s">
         <v>286</v>
@@ -7816,10 +7841,10 @@
         <v>43</v>
       </c>
       <c r="B53" s="58" t="s">
+        <v>422</v>
+      </c>
+      <c r="C53" s="59" t="s">
         <v>423</v>
-      </c>
-      <c r="C53" s="59" t="s">
-        <v>424</v>
       </c>
       <c r="D53" s="60">
         <v>1</v>
@@ -7828,7 +7853,7 @@
         <v>203</v>
       </c>
       <c r="F53" s="59" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="G53" s="36"/>
       <c r="H53" s="36" t="s">
@@ -7855,7 +7880,7 @@
       </c>
       <c r="N53" s="28"/>
       <c r="R53" s="36" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.2">
@@ -7863,16 +7888,16 @@
         <v>101</v>
       </c>
       <c r="B54" s="55" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="D54" s="38">
         <v>1</v>
       </c>
       <c r="F54" s="36" t="s">
+        <v>426</v>
+      </c>
+      <c r="G54" s="36" t="s">
         <v>427</v>
-      </c>
-      <c r="G54" s="36" t="s">
-        <v>428</v>
       </c>
       <c r="H54" s="36" t="s">
         <v>229</v>
@@ -7915,10 +7940,10 @@
         <v>203</v>
       </c>
       <c r="F55" s="36" t="s">
+        <v>428</v>
+      </c>
+      <c r="G55" s="37" t="s">
         <v>429</v>
-      </c>
-      <c r="G55" s="37" t="s">
-        <v>430</v>
       </c>
       <c r="H55" s="36" t="s">
         <v>229</v>
@@ -7949,10 +7974,10 @@
         <v>103</v>
       </c>
       <c r="B56" s="37" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C56" s="36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D56" s="38">
         <v>2</v>
@@ -7961,10 +7986,10 @@
         <v>203</v>
       </c>
       <c r="F56" s="36" t="s">
+        <v>335</v>
+      </c>
+      <c r="G56" s="36" t="s">
         <v>336</v>
-      </c>
-      <c r="G56" s="36" t="s">
-        <v>337</v>
       </c>
       <c r="H56" s="36" t="s">
         <v>206</v>
@@ -7990,7 +8015,7 @@
       </c>
       <c r="N56" s="28"/>
       <c r="R56" s="36" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="S56" s="36" t="s">
         <v>286</v>
@@ -8001,10 +8026,10 @@
         <v>104</v>
       </c>
       <c r="B57" s="36" t="s">
+        <v>430</v>
+      </c>
+      <c r="C57" s="37" t="s">
         <v>431</v>
-      </c>
-      <c r="C57" s="37" t="s">
-        <v>432</v>
       </c>
       <c r="D57" s="38">
         <v>1</v>
@@ -8013,10 +8038,10 @@
         <v>203</v>
       </c>
       <c r="F57" s="37" t="s">
+        <v>432</v>
+      </c>
+      <c r="G57" s="37" t="s">
         <v>433</v>
-      </c>
-      <c r="G57" s="37" t="s">
-        <v>434</v>
       </c>
       <c r="H57" s="36" t="s">
         <v>206</v>
@@ -8056,7 +8081,7 @@
         <v>203</v>
       </c>
       <c r="G58" s="37" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H58" s="36" t="s">
         <v>206</v>
@@ -8086,10 +8111,10 @@
         <v>106</v>
       </c>
       <c r="B59" s="36" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="C59" s="54" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="D59" s="38">
         <v>1</v>
@@ -8103,7 +8128,7 @@
         <v>107</v>
       </c>
       <c r="B60" s="56" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="J60" s="36">
         <f>IF(I60&gt;D60,0,D60-I60)</f>
@@ -8127,7 +8152,7 @@
         <v>108</v>
       </c>
       <c r="B61" s="56" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="J61" s="36">
         <f>IF(I61&gt;D61,0,D61-I61)</f>
@@ -8151,7 +8176,7 @@
         <v>109</v>
       </c>
       <c r="B62" s="56" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="J62" s="36">
         <f>IF(I62&gt;D62,0,D62-I62)</f>
@@ -8336,10 +8361,10 @@
         <v>301</v>
       </c>
       <c r="B7" s="36" t="s">
+        <v>435</v>
+      </c>
+      <c r="C7" s="37" t="s">
         <v>436</v>
-      </c>
-      <c r="C7" s="37" t="s">
-        <v>437</v>
       </c>
       <c r="D7" s="38">
         <v>1</v>
@@ -8349,7 +8374,7 @@
       </c>
       <c r="F7" s="37"/>
       <c r="G7" s="37" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="H7" s="36" t="s">
         <v>206</v>
@@ -8382,10 +8407,10 @@
         <v>302</v>
       </c>
       <c r="B8" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C8" s="45" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D8" s="38">
         <v>1</v>
@@ -8403,10 +8428,10 @@
         <v>303</v>
       </c>
       <c r="B9" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D9" s="38">
         <v>1</v>
@@ -8424,10 +8449,10 @@
         <v>304</v>
       </c>
       <c r="B10" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C10" s="47" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D10" s="49">
         <v>1</v>
@@ -8445,10 +8470,10 @@
         <v>305</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D11" s="38">
         <v>1</v>
@@ -8469,10 +8494,10 @@
         <v>306</v>
       </c>
       <c r="B12" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C12" s="47" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D12" s="49">
         <v>1</v>
@@ -8493,10 +8518,10 @@
         <v>307</v>
       </c>
       <c r="B13" s="48" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C13" s="47" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D13" s="49">
         <v>1</v>
@@ -8514,10 +8539,10 @@
         <v>308</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D14" s="38">
         <v>1</v>
@@ -8526,7 +8551,7 @@
         <v>203</v>
       </c>
       <c r="G14" s="45" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="H14" s="36" t="s">
         <v>206</v>
@@ -8556,10 +8581,10 @@
         <v>309</v>
       </c>
       <c r="B15" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C15" s="45" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="D15" s="38">
         <v>1</v>
@@ -8568,7 +8593,7 @@
         <v>203</v>
       </c>
       <c r="F15" s="46" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H15" s="36" t="s">
         <v>206</v>
@@ -8580,10 +8605,10 @@
         <v>310</v>
       </c>
       <c r="B16" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C16" s="45" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="D16" s="38">
         <v>1</v>
@@ -8592,7 +8617,7 @@
         <v>203</v>
       </c>
       <c r="F16" s="46" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H16" s="36" t="s">
         <v>206</v>
@@ -8604,13 +8629,13 @@
         <v>311</v>
       </c>
       <c r="B17" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="F17" s="46" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="H17" s="46" t="s">
         <v>206</v>
@@ -8622,10 +8647,10 @@
         <v>312</v>
       </c>
       <c r="B18" s="36" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D18" s="38">
         <v>1</v>
@@ -8634,7 +8659,7 @@
         <v>203</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="H18" s="46" t="s">
         <v>206</v>

</xml_diff>

<commit_message>
Core drive array assembled, LED array clear before serial wait.
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F29E46-7892-AF42-8283-A7924672B644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830A68FE-EA97-7E40-B70D-728408950366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="2160" windowWidth="32420" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="100" yWindow="2160" windowWidth="27140" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Concept Estimate" sheetId="1" r:id="rId1"/>
@@ -1758,9 +1758,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1772,6 +1769,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4569,11 +4569,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="61" t="s">
+      <c r="O3" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -5593,8 +5593,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B37" sqref="B37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5662,11 +5662,11 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="O7" s="61" t="s">
+      <c r="O7" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="P7" s="61"/>
-      <c r="Q7" s="61"/>
+      <c r="P7" s="65"/>
+      <c r="Q7" s="65"/>
     </row>
     <row r="8" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -5932,7 +5932,7 @@
       <c r="A13" s="36">
         <v>3</v>
       </c>
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="58" t="s">
         <v>289</v>
       </c>
       <c r="C13" s="36" t="s">
@@ -5999,10 +5999,10 @@
       <c r="E14" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F14" s="62" t="s">
+      <c r="F14" s="61" t="s">
         <v>459</v>
       </c>
-      <c r="G14" s="63" t="s">
+      <c r="G14" s="62" t="s">
         <v>294</v>
       </c>
       <c r="H14" s="36" t="s">
@@ -6278,10 +6278,10 @@
       <c r="E20" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="63" t="s">
+      <c r="F20" s="62" t="s">
         <v>311</v>
       </c>
-      <c r="G20" s="63" t="s">
+      <c r="G20" s="62" t="s">
         <v>312</v>
       </c>
       <c r="H20" s="36" t="s">
@@ -6334,13 +6334,13 @@
       <c r="A21" s="36">
         <v>11</v>
       </c>
-      <c r="B21" s="64" t="s">
+      <c r="B21" s="63" t="s">
         <v>318</v>
       </c>
       <c r="C21" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="D21" s="65">
+      <c r="D21" s="64">
         <v>1</v>
       </c>
       <c r="E21" s="40" t="s">
@@ -7118,7 +7118,7 @@
       <c r="A39" s="36">
         <v>29</v>
       </c>
-      <c r="B39" s="37" t="s">
+      <c r="B39" s="58" t="s">
         <v>366</v>
       </c>
       <c r="C39" s="36" t="s">
@@ -7170,7 +7170,7 @@
       <c r="A40" s="36">
         <v>30</v>
       </c>
-      <c r="B40" s="37" t="s">
+      <c r="B40" s="58" t="s">
         <v>368</v>
       </c>
       <c r="C40" s="36" t="s">
@@ -7222,7 +7222,7 @@
       <c r="A41" s="36">
         <v>31</v>
       </c>
-      <c r="B41" s="37" t="s">
+      <c r="B41" s="58" t="s">
         <v>370</v>
       </c>
       <c r="C41" s="36" t="s">
@@ -7632,7 +7632,7 @@
       <c r="A49" s="36">
         <v>39</v>
       </c>
-      <c r="B49" s="37" t="s">
+      <c r="B49" s="58" t="s">
         <v>247</v>
       </c>
       <c r="C49" s="36" t="s">
@@ -7684,7 +7684,7 @@
       <c r="A50" s="36">
         <v>40</v>
       </c>
-      <c r="B50" s="37" t="s">
+      <c r="B50" s="58" t="s">
         <v>249</v>
       </c>
       <c r="C50" s="36" t="s">
@@ -8249,11 +8249,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="61" t="s">
+      <c r="O3" s="65" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="61"/>
-      <c r="Q3" s="61"/>
+      <c r="P3" s="65"/>
+      <c r="Q3" s="65"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>

</xml_diff>

<commit_message>
BOM assembly progress highlight updates.
</commit_message>
<xml_diff>
--- a/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
+++ b/Manufacturing/BOM Core 64 v0.3.0 Red Dual Boards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ageppert/Dropbox/Electronics/Core 64 Interactive Badge/Core-64-Interactive-Core-Memory-Badge/Manufacturing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{830A68FE-EA97-7E40-B70D-728408950366}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F921C05D-F22C-604D-A018-A0D077698932}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="100" yWindow="2160" windowWidth="27140" windowHeight="20000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1395,9 +1395,6 @@
     <t>Glue magnet to stylus</t>
   </si>
   <si>
-    <t>Lanyard</t>
-  </si>
-  <si>
     <t>Not labeled - for Adafruit MicroSD Breakout</t>
   </si>
   <si>
@@ -1423,6 +1420,9 @@
   </si>
   <si>
     <t>MBR120 CHANGE?? S1M-13-F</t>
+  </si>
+  <si>
+    <t>Lanyard, or alligator clip test leads. 26-28" OAL w/clips</t>
   </si>
 </sst>
 </file>
@@ -1434,10 +1434,17 @@
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0.0000_);_(&quot;$&quot;* \(#,##0.0000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0.000_);_(&quot;$&quot;* \(#,##0.000\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
@@ -1616,36 +1623,36 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="9" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="8" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="44" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="44" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1655,123 +1662,126 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="44" fontId="0" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="11" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="10" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="44" fontId="12" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="44" fontId="11" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="11" fillId="0" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4569,11 +4579,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="65" t="s">
+      <c r="O3" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -5327,7 +5337,7 @@
       <c r="E20" s="28" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="57" t="s">
+      <c r="F20" s="56" t="s">
         <v>244</v>
       </c>
       <c r="H20" s="28" t="s">
@@ -5593,8 +5603,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1052A41E-3EA7-B148-953B-E2218E71D84C}">
   <dimension ref="A1:AD62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+    <sheetView tabSelected="1" topLeftCell="A36" zoomScale="125" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5662,11 +5672,11 @@
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="O7" s="65" t="s">
+      <c r="O7" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="65"/>
+      <c r="P7" s="64"/>
+      <c r="Q7" s="64"/>
     </row>
     <row r="8" spans="1:30" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="36" t="s">
@@ -5820,7 +5830,7 @@
       <c r="A11" s="36">
         <v>1</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="57" t="s">
         <v>281</v>
       </c>
       <c r="C11" s="36" t="s">
@@ -5876,7 +5886,7 @@
       <c r="A12" s="36">
         <v>2</v>
       </c>
-      <c r="B12" s="58" t="s">
+      <c r="B12" s="57" t="s">
         <v>287</v>
       </c>
       <c r="C12" s="36" t="s">
@@ -5932,7 +5942,7 @@
       <c r="A13" s="36">
         <v>3</v>
       </c>
-      <c r="B13" s="58" t="s">
+      <c r="B13" s="57" t="s">
         <v>289</v>
       </c>
       <c r="C13" s="36" t="s">
@@ -5987,22 +5997,22 @@
       <c r="A14" s="36">
         <v>4</v>
       </c>
-      <c r="B14" s="58" t="s">
+      <c r="B14" s="57" t="s">
         <v>292</v>
       </c>
-      <c r="C14" s="59" t="s">
+      <c r="C14" s="58" t="s">
         <v>293</v>
       </c>
-      <c r="D14" s="60">
+      <c r="D14" s="59">
         <v>1</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F14" s="61" t="s">
-        <v>459</v>
-      </c>
-      <c r="G14" s="62" t="s">
+      <c r="F14" s="60" t="s">
+        <v>458</v>
+      </c>
+      <c r="G14" s="61" t="s">
         <v>294</v>
       </c>
       <c r="H14" s="36" t="s">
@@ -6046,7 +6056,7 @@
       <c r="A15" s="36">
         <v>5</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="57" t="s">
         <v>297</v>
       </c>
       <c r="C15" s="36" t="s">
@@ -6106,7 +6116,7 @@
       <c r="A16" s="36">
         <v>6</v>
       </c>
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="57" t="s">
         <v>302</v>
       </c>
       <c r="C16" s="36" t="s">
@@ -6166,19 +6176,19 @@
       <c r="A17" s="36">
         <v>7</v>
       </c>
-      <c r="B17" s="58" t="s">
+      <c r="B17" s="57" t="s">
         <v>305</v>
       </c>
-      <c r="C17" s="59" t="s">
+      <c r="C17" s="58" t="s">
         <v>306</v>
       </c>
-      <c r="D17" s="60">
+      <c r="D17" s="59">
         <v>1</v>
       </c>
       <c r="E17" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F17" s="59" t="s">
+      <c r="F17" s="58" t="s">
         <v>307</v>
       </c>
       <c r="G17" s="36" t="s">
@@ -6266,22 +6276,22 @@
       <c r="A20" s="36">
         <v>10</v>
       </c>
-      <c r="B20" s="58" t="s">
+      <c r="B20" s="57" t="s">
         <v>309</v>
       </c>
-      <c r="C20" s="59" t="s">
+      <c r="C20" s="58" t="s">
         <v>310</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="59">
         <v>1</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F20" s="62" t="s">
+      <c r="F20" s="61" t="s">
         <v>311</v>
       </c>
-      <c r="G20" s="62" t="s">
+      <c r="G20" s="61" t="s">
         <v>312</v>
       </c>
       <c r="H20" s="36" t="s">
@@ -6334,13 +6344,13 @@
       <c r="A21" s="36">
         <v>11</v>
       </c>
-      <c r="B21" s="63" t="s">
+      <c r="B21" s="62" t="s">
         <v>318</v>
       </c>
       <c r="C21" s="39" t="s">
         <v>319</v>
       </c>
-      <c r="D21" s="64">
+      <c r="D21" s="63">
         <v>1</v>
       </c>
       <c r="E21" s="40" t="s">
@@ -6390,7 +6400,7 @@
       <c r="A22" s="36">
         <v>12</v>
       </c>
-      <c r="B22" s="58" t="s">
+      <c r="B22" s="57" t="s">
         <v>323</v>
       </c>
       <c r="C22" s="36" t="s">
@@ -6446,7 +6456,7 @@
       <c r="A23" s="36">
         <v>13</v>
       </c>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="57" t="s">
         <v>328</v>
       </c>
       <c r="C23" s="36" t="s">
@@ -6664,19 +6674,19 @@
       <c r="A31" s="36">
         <v>21</v>
       </c>
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="57" t="s">
         <v>338</v>
       </c>
-      <c r="C31" s="59" t="s">
+      <c r="C31" s="58" t="s">
         <v>339</v>
       </c>
-      <c r="D31" s="60">
+      <c r="D31" s="59">
         <v>1</v>
       </c>
       <c r="E31" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F31" s="59" t="s">
+      <c r="F31" s="58" t="s">
         <v>340</v>
       </c>
       <c r="G31" s="36" t="s">
@@ -6716,7 +6726,7 @@
       <c r="A32" s="36">
         <v>22</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="57" t="s">
         <v>344</v>
       </c>
       <c r="C32" s="36" t="s">
@@ -6791,7 +6801,7 @@
       <c r="A33" s="36">
         <v>23</v>
       </c>
-      <c r="B33" s="37" t="s">
+      <c r="B33" s="57" t="s">
         <v>352</v>
       </c>
       <c r="C33" s="36" t="s">
@@ -6866,19 +6876,19 @@
       <c r="A34" s="36">
         <v>24</v>
       </c>
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="57" t="s">
         <v>356</v>
       </c>
-      <c r="C34" s="59" t="s">
+      <c r="C34" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="D34" s="60">
+      <c r="D34" s="59">
         <v>1</v>
       </c>
       <c r="E34" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F34" s="59">
+      <c r="F34" s="58">
         <v>0.1</v>
       </c>
       <c r="G34" s="36"/>
@@ -6916,19 +6926,19 @@
       <c r="A35" s="36">
         <v>25</v>
       </c>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="57" t="s">
         <v>359</v>
       </c>
-      <c r="C35" s="59" t="s">
+      <c r="C35" s="58" t="s">
         <v>357</v>
       </c>
-      <c r="D35" s="60">
+      <c r="D35" s="59">
         <v>2</v>
       </c>
       <c r="E35" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F35" s="59" t="s">
+      <c r="F35" s="58" t="s">
         <v>234</v>
       </c>
       <c r="G35" s="36" t="s">
@@ -6967,7 +6977,7 @@
       <c r="A36" s="36">
         <v>26</v>
       </c>
-      <c r="B36" s="58" t="s">
+      <c r="B36" s="57" t="s">
         <v>360</v>
       </c>
       <c r="C36" s="36" t="s">
@@ -7016,7 +7026,7 @@
       <c r="A37" s="36">
         <v>27</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="57" t="s">
         <v>362</v>
       </c>
       <c r="C37" s="36" t="s">
@@ -7067,7 +7077,7 @@
       <c r="A38" s="36">
         <v>28</v>
       </c>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="57" t="s">
         <v>364</v>
       </c>
       <c r="C38" s="36" t="s">
@@ -7118,7 +7128,7 @@
       <c r="A39" s="36">
         <v>29</v>
       </c>
-      <c r="B39" s="58" t="s">
+      <c r="B39" s="57" t="s">
         <v>366</v>
       </c>
       <c r="C39" s="36" t="s">
@@ -7170,7 +7180,7 @@
       <c r="A40" s="36">
         <v>30</v>
       </c>
-      <c r="B40" s="58" t="s">
+      <c r="B40" s="57" t="s">
         <v>368</v>
       </c>
       <c r="C40" s="36" t="s">
@@ -7222,7 +7232,7 @@
       <c r="A41" s="36">
         <v>31</v>
       </c>
-      <c r="B41" s="58" t="s">
+      <c r="B41" s="57" t="s">
         <v>370</v>
       </c>
       <c r="C41" s="36" t="s">
@@ -7273,7 +7283,7 @@
       <c r="A42" s="36">
         <v>32</v>
       </c>
-      <c r="B42" s="58" t="s">
+      <c r="B42" s="57" t="s">
         <v>372</v>
       </c>
       <c r="C42" s="36" t="s">
@@ -7325,19 +7335,19 @@
       <c r="A43" s="36">
         <v>33</v>
       </c>
-      <c r="B43" s="58" t="s">
+      <c r="B43" s="57" t="s">
         <v>374</v>
       </c>
-      <c r="C43" s="59" t="s">
+      <c r="C43" s="58" t="s">
         <v>375</v>
       </c>
-      <c r="D43" s="60">
+      <c r="D43" s="59">
         <v>1</v>
       </c>
       <c r="E43" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F43" s="59" t="s">
+      <c r="F43" s="58" t="s">
         <v>376</v>
       </c>
       <c r="G43" s="36" t="s">
@@ -7377,19 +7387,19 @@
       <c r="A44" s="36">
         <v>34</v>
       </c>
-      <c r="B44" s="58" t="s">
+      <c r="B44" s="57" t="s">
         <v>235</v>
       </c>
-      <c r="C44" s="59" t="s">
+      <c r="C44" s="58" t="s">
         <v>379</v>
       </c>
-      <c r="D44" s="60">
+      <c r="D44" s="59">
         <v>1</v>
       </c>
       <c r="E44" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F44" s="59" t="s">
+      <c r="F44" s="58" t="s">
         <v>380</v>
       </c>
       <c r="G44" s="36" t="s">
@@ -7429,19 +7439,19 @@
       <c r="A45" s="36">
         <v>35</v>
       </c>
-      <c r="B45" s="58" t="s">
+      <c r="B45" s="57" t="s">
         <v>384</v>
       </c>
-      <c r="C45" s="59" t="s">
+      <c r="C45" s="58" t="s">
         <v>385</v>
       </c>
-      <c r="D45" s="60">
+      <c r="D45" s="59">
         <v>1</v>
       </c>
       <c r="E45" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F45" s="59" t="s">
+      <c r="F45" s="58" t="s">
         <v>137</v>
       </c>
       <c r="G45" s="36"/>
@@ -7476,19 +7486,19 @@
       <c r="A46" s="36">
         <v>36</v>
       </c>
-      <c r="B46" s="58" t="s">
+      <c r="B46" s="57" t="s">
         <v>240</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="C46" s="58" t="s">
         <v>387</v>
       </c>
-      <c r="D46" s="60">
+      <c r="D46" s="59">
         <v>1</v>
       </c>
       <c r="E46" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F46" s="59" t="s">
+      <c r="F46" s="58" t="s">
         <v>388</v>
       </c>
       <c r="G46" s="36" t="s">
@@ -7528,7 +7538,7 @@
       <c r="A47" s="36">
         <v>37</v>
       </c>
-      <c r="B47" s="58" t="s">
+      <c r="B47" s="57" t="s">
         <v>392</v>
       </c>
       <c r="C47" s="36" t="s">
@@ -7580,7 +7590,7 @@
       <c r="A48" s="36">
         <v>38</v>
       </c>
-      <c r="B48" s="58" t="s">
+      <c r="B48" s="57" t="s">
         <v>398</v>
       </c>
       <c r="C48" s="36" t="s">
@@ -7632,7 +7642,7 @@
       <c r="A49" s="36">
         <v>39</v>
       </c>
-      <c r="B49" s="58" t="s">
+      <c r="B49" s="57" t="s">
         <v>247</v>
       </c>
       <c r="C49" s="36" t="s">
@@ -7684,7 +7694,7 @@
       <c r="A50" s="36">
         <v>40</v>
       </c>
-      <c r="B50" s="58" t="s">
+      <c r="B50" s="57" t="s">
         <v>249</v>
       </c>
       <c r="C50" s="36" t="s">
@@ -7736,19 +7746,19 @@
       <c r="A51" s="36">
         <v>41</v>
       </c>
-      <c r="B51" s="58" t="s">
+      <c r="B51" s="57" t="s">
         <v>251</v>
       </c>
-      <c r="C51" s="59" t="s">
+      <c r="C51" s="58" t="s">
         <v>413</v>
       </c>
-      <c r="D51" s="60">
+      <c r="D51" s="59">
         <v>1</v>
       </c>
       <c r="E51" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F51" s="59" t="s">
+      <c r="F51" s="58" t="s">
         <v>414</v>
       </c>
       <c r="G51" s="37" t="s">
@@ -7788,7 +7798,7 @@
       <c r="A52" s="36">
         <v>42</v>
       </c>
-      <c r="B52" s="58" t="s">
+      <c r="B52" s="57" t="s">
         <v>417</v>
       </c>
       <c r="C52" s="36" t="s">
@@ -7840,19 +7850,19 @@
       <c r="A53" s="36">
         <v>43</v>
       </c>
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="57" t="s">
         <v>422</v>
       </c>
-      <c r="C53" s="59" t="s">
+      <c r="C53" s="58" t="s">
         <v>423</v>
       </c>
-      <c r="D53" s="60">
+      <c r="D53" s="59">
         <v>1</v>
       </c>
       <c r="E53" s="30" t="s">
         <v>203</v>
       </c>
-      <c r="F53" s="59" t="s">
+      <c r="F53" s="58" t="s">
         <v>424</v>
       </c>
       <c r="G53" s="36"/>
@@ -7887,8 +7897,8 @@
       <c r="A54" s="36">
         <v>101</v>
       </c>
-      <c r="B54" s="55" t="s">
-        <v>451</v>
+      <c r="B54" s="54" t="s">
+        <v>450</v>
       </c>
       <c r="D54" s="38">
         <v>1</v>
@@ -8070,11 +8080,11 @@
       <c r="A58" s="36">
         <v>105</v>
       </c>
-      <c r="B58" s="59" t="s">
+      <c r="B58" s="58" t="s">
         <v>142</v>
       </c>
-      <c r="C58" s="58"/>
-      <c r="D58" s="60">
+      <c r="C58" s="57"/>
+      <c r="D58" s="59">
         <v>1</v>
       </c>
       <c r="E58" s="30" t="s">
@@ -8110,11 +8120,11 @@
       <c r="A59" s="36">
         <v>106</v>
       </c>
-      <c r="B59" s="36" t="s">
-        <v>430</v>
-      </c>
-      <c r="C59" s="54" t="s">
-        <v>450</v>
+      <c r="B59" s="65" t="s">
+        <v>435</v>
+      </c>
+      <c r="C59" s="66" t="s">
+        <v>459</v>
       </c>
       <c r="D59" s="38">
         <v>1</v>
@@ -8127,8 +8137,8 @@
       <c r="A60" s="36">
         <v>107</v>
       </c>
-      <c r="B60" s="56" t="s">
-        <v>456</v>
+      <c r="B60" s="55" t="s">
+        <v>455</v>
       </c>
       <c r="J60" s="36">
         <f>IF(I60&gt;D60,0,D60-I60)</f>
@@ -8151,8 +8161,8 @@
       <c r="A61" s="36">
         <v>108</v>
       </c>
-      <c r="B61" s="56" t="s">
-        <v>457</v>
+      <c r="B61" s="55" t="s">
+        <v>456</v>
       </c>
       <c r="J61" s="36">
         <f>IF(I61&gt;D61,0,D61-I61)</f>
@@ -8175,8 +8185,8 @@
       <c r="A62" s="36">
         <v>109</v>
       </c>
-      <c r="B62" s="56" t="s">
-        <v>458</v>
+      <c r="B62" s="55" t="s">
+        <v>457</v>
       </c>
       <c r="J62" s="36">
         <f>IF(I62&gt;D62,0,D62-I62)</f>
@@ -8249,11 +8259,11 @@
       <c r="B3" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="O3" s="65" t="s">
+      <c r="O3" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="65"/>
+      <c r="P3" s="64"/>
+      <c r="Q3" s="64"/>
     </row>
     <row r="4" spans="1:17" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="29"/>
@@ -8593,7 +8603,7 @@
         <v>203</v>
       </c>
       <c r="F15" s="46" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H15" s="36" t="s">
         <v>206</v>
@@ -8617,7 +8627,7 @@
         <v>203</v>
       </c>
       <c r="F16" s="46" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="H16" s="36" t="s">
         <v>206</v>
@@ -8635,7 +8645,7 @@
         <v>449</v>
       </c>
       <c r="F17" s="46" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="H17" s="46" t="s">
         <v>206</v>
@@ -8650,7 +8660,7 @@
         <v>435</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D18" s="38">
         <v>1</v>
@@ -8659,7 +8669,7 @@
         <v>203</v>
       </c>
       <c r="F18" s="46" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="H18" s="46" t="s">
         <v>206</v>

</xml_diff>